<commit_message>
Fixed the bug where numbers from Twitter exports were being written to the completed sheet as strings. Also fixed the bug where the first line of the Twitter export was being written to the completed sheet even though it is just a header. Added: program now searches for '&amp;' in the caption and replaces it with '&'.
</commit_message>
<xml_diff>
--- a/files/SodexoSheetTemplate.xlsx
+++ b/files/SodexoSheetTemplate.xlsx
@@ -522,18 +522,18 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" customWidth="1"/>
-    <col min="3" max="3" width="98.1640625" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="104.5" customWidth="1"/>
     <col min="4" max="4" width="10.1640625" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="54.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="17" width="6.6640625" customWidth="1"/>
     <col min="18" max="26" width="13.1640625" customWidth="1"/>
   </cols>
@@ -580,7 +580,7 @@
       <c r="Y1" s="6"/>
       <c r="Z1" s="6"/>
     </row>
-    <row r="2" spans="1:26" ht="30" customHeight="1">
+    <row r="2" spans="1:26" ht="14">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="9"/>
@@ -608,7 +608,7 @@
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
     </row>
-    <row r="3" spans="1:26" ht="30" customHeight="1">
+    <row r="3" spans="1:26" ht="14">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
@@ -664,7 +664,7 @@
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
     </row>
-    <row r="5" spans="1:26" ht="30" customHeight="1">
+    <row r="5" spans="1:26" ht="14">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
@@ -692,7 +692,7 @@
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
     </row>
-    <row r="6" spans="1:26" ht="30" customHeight="1">
+    <row r="6" spans="1:26" ht="14">
       <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
@@ -720,7 +720,7 @@
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
     </row>
-    <row r="7" spans="1:26" ht="30" customHeight="1">
+    <row r="7" spans="1:26" ht="14">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
@@ -776,7 +776,7 @@
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
     </row>
-    <row r="9" spans="1:26" ht="30" customHeight="1">
+    <row r="9" spans="1:26" ht="14">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
@@ -832,7 +832,7 @@
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
     </row>
-    <row r="11" spans="1:26" ht="30" customHeight="1">
+    <row r="11" spans="1:26" ht="14">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
@@ -1056,7 +1056,7 @@
       <c r="Y18" s="6"/>
       <c r="Z18" s="6"/>
     </row>
-    <row r="19" spans="1:26" ht="30" customHeight="1">
+    <row r="19" spans="1:26" ht="14">
       <c r="A19" s="12"/>
       <c r="B19" s="13"/>
       <c r="C19" s="14"/>
@@ -1168,7 +1168,7 @@
       <c r="Y22" s="6"/>
       <c r="Z22" s="6"/>
     </row>
-    <row r="23" spans="1:26" ht="30" customHeight="1">
+    <row r="23" spans="1:26" ht="14">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="9"/>
@@ -1196,7 +1196,7 @@
       <c r="Y23" s="6"/>
       <c r="Z23" s="6"/>
     </row>
-    <row r="24" spans="1:26" ht="30" customHeight="1">
+    <row r="24" spans="1:26" ht="14">
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
@@ -1224,7 +1224,7 @@
       <c r="Y24" s="6"/>
       <c r="Z24" s="6"/>
     </row>
-    <row r="25" spans="1:26" ht="30" customHeight="1">
+    <row r="25" spans="1:26" ht="14">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
@@ -1252,7 +1252,7 @@
       <c r="Y25" s="6"/>
       <c r="Z25" s="6"/>
     </row>
-    <row r="26" spans="1:26" ht="30" customHeight="1">
+    <row r="26" spans="1:26" ht="14">
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
@@ -1336,7 +1336,7 @@
       <c r="Y28" s="6"/>
       <c r="Z28" s="6"/>
     </row>
-    <row r="29" spans="1:26" ht="30" customHeight="1">
+    <row r="29" spans="1:26" ht="14">
       <c r="A29" s="7"/>
       <c r="B29" s="8"/>
       <c r="C29" s="9"/>
@@ -1364,7 +1364,7 @@
       <c r="Y29" s="6"/>
       <c r="Z29" s="6"/>
     </row>
-    <row r="30" spans="1:26" ht="30" customHeight="1">
+    <row r="30" spans="1:26" ht="14">
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="9"/>
@@ -1504,7 +1504,7 @@
       <c r="Y34" s="6"/>
       <c r="Z34" s="6"/>
     </row>
-    <row r="35" spans="1:26" ht="30" customHeight="1">
+    <row r="35" spans="1:26" ht="14">
       <c r="A35" s="12"/>
       <c r="B35" s="13"/>
       <c r="C35" s="14"/>
@@ -1532,7 +1532,7 @@
       <c r="Y35" s="6"/>
       <c r="Z35" s="6"/>
     </row>
-    <row r="36" spans="1:26" ht="30" customHeight="1">
+    <row r="36" spans="1:26" ht="14">
       <c r="A36" s="12"/>
       <c r="B36" s="13"/>
       <c r="C36" s="14"/>
@@ -1588,7 +1588,7 @@
       <c r="Y37" s="6"/>
       <c r="Z37" s="6"/>
     </row>
-    <row r="38" spans="1:26" ht="30" customHeight="1">
+    <row r="38" spans="1:26" ht="14">
       <c r="A38" s="12"/>
       <c r="B38" s="13"/>
       <c r="C38" s="14"/>
@@ -1644,7 +1644,7 @@
       <c r="Y39" s="6"/>
       <c r="Z39" s="6"/>
     </row>
-    <row r="40" spans="1:26" ht="30" customHeight="1">
+    <row r="40" spans="1:26" ht="14">
       <c r="A40" s="7"/>
       <c r="B40" s="8"/>
       <c r="C40" s="9"/>
@@ -1924,7 +1924,7 @@
       <c r="Y49" s="6"/>
       <c r="Z49" s="6"/>
     </row>
-    <row r="50" spans="1:26" ht="30" customHeight="1">
+    <row r="50" spans="1:26" ht="14">
       <c r="A50" s="7"/>
       <c r="B50" s="8"/>
       <c r="C50" s="9"/>
@@ -1952,7 +1952,7 @@
       <c r="Y50" s="6"/>
       <c r="Z50" s="6"/>
     </row>
-    <row r="51" spans="1:26" ht="30" customHeight="1">
+    <row r="51" spans="1:26" ht="14">
       <c r="A51" s="7"/>
       <c r="B51" s="8"/>
       <c r="C51" s="9"/>
@@ -2008,7 +2008,7 @@
       <c r="Y52" s="6"/>
       <c r="Z52" s="6"/>
     </row>
-    <row r="53" spans="1:26" ht="30" customHeight="1">
+    <row r="53" spans="1:26" ht="14">
       <c r="A53" s="7"/>
       <c r="B53" s="8"/>
       <c r="C53" s="9"/>
@@ -2064,7 +2064,7 @@
       <c r="Y54" s="6"/>
       <c r="Z54" s="6"/>
     </row>
-    <row r="55" spans="1:26" ht="30" customHeight="1">
+    <row r="55" spans="1:26" ht="14">
       <c r="A55" s="7"/>
       <c r="B55" s="8"/>
       <c r="C55" s="9"/>
@@ -2120,7 +2120,7 @@
       <c r="Y56" s="6"/>
       <c r="Z56" s="6"/>
     </row>
-    <row r="57" spans="1:26" ht="30" customHeight="1">
+    <row r="57" spans="1:26" ht="14">
       <c r="A57" s="7"/>
       <c r="B57" s="8"/>
       <c r="C57" s="9"/>
@@ -2176,7 +2176,7 @@
       <c r="Y58" s="6"/>
       <c r="Z58" s="6"/>
     </row>
-    <row r="59" spans="1:26" ht="30" customHeight="1">
+    <row r="59" spans="1:26" ht="14">
       <c r="A59" s="12"/>
       <c r="B59" s="13"/>
       <c r="C59" s="14"/>
@@ -2372,7 +2372,7 @@
       <c r="Y65" s="6"/>
       <c r="Z65" s="6"/>
     </row>
-    <row r="66" spans="1:26" ht="30" customHeight="1">
+    <row r="66" spans="1:26" ht="14">
       <c r="A66" s="12"/>
       <c r="B66" s="13"/>
       <c r="C66" s="14"/>
@@ -2568,7 +2568,7 @@
       <c r="Y72" s="6"/>
       <c r="Z72" s="6"/>
     </row>
-    <row r="73" spans="1:26" ht="30" customHeight="1">
+    <row r="73" spans="1:26" ht="14">
       <c r="A73" s="7"/>
       <c r="B73" s="8"/>
       <c r="C73" s="9"/>
@@ -2652,7 +2652,7 @@
       <c r="Y75" s="6"/>
       <c r="Z75" s="6"/>
     </row>
-    <row r="76" spans="1:26" ht="30" customHeight="1">
+    <row r="76" spans="1:26" ht="14">
       <c r="A76" s="7"/>
       <c r="B76" s="8"/>
       <c r="C76" s="9"/>
@@ -2736,7 +2736,7 @@
       <c r="Y78" s="6"/>
       <c r="Z78" s="6"/>
     </row>
-    <row r="79" spans="1:26" ht="30" customHeight="1">
+    <row r="79" spans="1:26" ht="14">
       <c r="A79" s="7"/>
       <c r="B79" s="8"/>
       <c r="C79" s="9"/>
@@ -2848,7 +2848,7 @@
       <c r="Y82" s="6"/>
       <c r="Z82" s="6"/>
     </row>
-    <row r="83" spans="1:26" ht="30" customHeight="1">
+    <row r="83" spans="1:26" ht="14">
       <c r="A83" s="7"/>
       <c r="B83" s="8"/>
       <c r="C83" s="9"/>
@@ -2876,7 +2876,7 @@
       <c r="Y83" s="6"/>
       <c r="Z83" s="6"/>
     </row>
-    <row r="84" spans="1:26" ht="30" customHeight="1">
+    <row r="84" spans="1:26" ht="14">
       <c r="A84" s="7"/>
       <c r="B84" s="8"/>
       <c r="C84" s="9"/>
@@ -2932,7 +2932,7 @@
       <c r="Y85" s="6"/>
       <c r="Z85" s="6"/>
     </row>
-    <row r="86" spans="1:26" ht="30" customHeight="1">
+    <row r="86" spans="1:26" ht="14">
       <c r="A86" s="7"/>
       <c r="B86" s="8"/>
       <c r="C86" s="9"/>
@@ -2988,7 +2988,7 @@
       <c r="Y87" s="6"/>
       <c r="Z87" s="6"/>
     </row>
-    <row r="88" spans="1:26" ht="30" customHeight="1">
+    <row r="88" spans="1:26" ht="14">
       <c r="A88" s="7"/>
       <c r="B88" s="8"/>
       <c r="C88" s="9"/>
@@ -3044,7 +3044,7 @@
       <c r="Y89" s="6"/>
       <c r="Z89" s="6"/>
     </row>
-    <row r="90" spans="1:26" ht="30" customHeight="1">
+    <row r="90" spans="1:26" ht="14">
       <c r="A90" s="7"/>
       <c r="B90" s="8"/>
       <c r="C90" s="9"/>
@@ -3184,7 +3184,7 @@
       <c r="Y94" s="6"/>
       <c r="Z94" s="6"/>
     </row>
-    <row r="95" spans="1:26" ht="30" customHeight="1">
+    <row r="95" spans="1:26" ht="14">
       <c r="A95" s="12"/>
       <c r="B95" s="13"/>
       <c r="C95" s="14"/>
@@ -3380,7 +3380,7 @@
       <c r="Y101" s="6"/>
       <c r="Z101" s="6"/>
     </row>
-    <row r="102" spans="1:26" ht="30" customHeight="1">
+    <row r="102" spans="1:26" ht="14">
       <c r="A102" s="7"/>
       <c r="B102" s="8"/>
       <c r="C102" s="9"/>
@@ -3688,7 +3688,7 @@
       <c r="Y112" s="6"/>
       <c r="Z112" s="6"/>
     </row>
-    <row r="113" spans="1:26" ht="30" customHeight="1">
+    <row r="113" spans="1:26" ht="14">
       <c r="A113" s="7"/>
       <c r="B113" s="8"/>
       <c r="C113" s="9"/>
@@ -3772,7 +3772,7 @@
       <c r="Y115" s="6"/>
       <c r="Z115" s="6"/>
     </row>
-    <row r="116" spans="1:26" ht="30" customHeight="1">
+    <row r="116" spans="1:26" ht="14">
       <c r="A116" s="7"/>
       <c r="B116" s="8"/>
       <c r="C116" s="9"/>
@@ -3800,7 +3800,7 @@
       <c r="Y116" s="6"/>
       <c r="Z116" s="6"/>
     </row>
-    <row r="117" spans="1:26" ht="30" customHeight="1">
+    <row r="117" spans="1:26" ht="14">
       <c r="A117" s="7"/>
       <c r="B117" s="8"/>
       <c r="C117" s="9"/>
@@ -3828,7 +3828,7 @@
       <c r="Y117" s="6"/>
       <c r="Z117" s="6"/>
     </row>
-    <row r="118" spans="1:26" ht="30" customHeight="1">
+    <row r="118" spans="1:26" ht="14">
       <c r="A118" s="7"/>
       <c r="B118" s="8"/>
       <c r="C118" s="9"/>
@@ -3968,7 +3968,7 @@
       <c r="Y122" s="6"/>
       <c r="Z122" s="6"/>
     </row>
-    <row r="123" spans="1:26" ht="30" customHeight="1">
+    <row r="123" spans="1:26" ht="14">
       <c r="A123" s="7"/>
       <c r="B123" s="8"/>
       <c r="C123" s="9"/>
@@ -3996,7 +3996,7 @@
       <c r="Y123" s="6"/>
       <c r="Z123" s="6"/>
     </row>
-    <row r="124" spans="1:26" ht="30" customHeight="1">
+    <row r="124" spans="1:26" ht="14">
       <c r="A124" s="7"/>
       <c r="B124" s="8"/>
       <c r="C124" s="9"/>
@@ -4080,7 +4080,7 @@
       <c r="Y126" s="6"/>
       <c r="Z126" s="6"/>
     </row>
-    <row r="127" spans="1:26" ht="30" customHeight="1">
+    <row r="127" spans="1:26" ht="14">
       <c r="A127" s="7"/>
       <c r="B127" s="8"/>
       <c r="C127" s="9"/>
@@ -4220,7 +4220,7 @@
       <c r="Y131" s="6"/>
       <c r="Z131" s="6"/>
     </row>
-    <row r="132" spans="1:26" ht="30" customHeight="1">
+    <row r="132" spans="1:26" ht="14">
       <c r="A132" s="7"/>
       <c r="B132" s="8"/>
       <c r="C132" s="9"/>
@@ -4248,7 +4248,7 @@
       <c r="Y132" s="6"/>
       <c r="Z132" s="6"/>
     </row>
-    <row r="133" spans="1:26" ht="150" customHeight="1">
+    <row r="133" spans="1:26" ht="14">
       <c r="A133" s="12"/>
       <c r="B133" s="13"/>
       <c r="C133" s="14"/>
@@ -4276,7 +4276,7 @@
       <c r="Y133" s="6"/>
       <c r="Z133" s="6"/>
     </row>
-    <row r="134" spans="1:26" ht="30" customHeight="1">
+    <row r="134" spans="1:26" ht="14">
       <c r="A134" s="12"/>
       <c r="B134" s="13"/>
       <c r="C134" s="14"/>
@@ -4388,7 +4388,7 @@
       <c r="Y137" s="6"/>
       <c r="Z137" s="6"/>
     </row>
-    <row r="138" spans="1:26" ht="30" customHeight="1">
+    <row r="138" spans="1:26" ht="14">
       <c r="A138" s="12"/>
       <c r="B138" s="13"/>
       <c r="C138" s="14"/>
@@ -4444,7 +4444,7 @@
       <c r="Y139" s="6"/>
       <c r="Z139" s="6"/>
     </row>
-    <row r="140" spans="1:26" ht="30" customHeight="1">
+    <row r="140" spans="1:26" ht="14">
       <c r="A140" s="7"/>
       <c r="B140" s="8"/>
       <c r="C140" s="9"/>
@@ -4556,7 +4556,7 @@
       <c r="Y143" s="6"/>
       <c r="Z143" s="6"/>
     </row>
-    <row r="144" spans="1:26" ht="30" customHeight="1">
+    <row r="144" spans="1:26" ht="14">
       <c r="A144" s="7"/>
       <c r="B144" s="8"/>
       <c r="C144" s="9"/>
@@ -4612,7 +4612,7 @@
       <c r="Y145" s="6"/>
       <c r="Z145" s="6"/>
     </row>
-    <row r="146" spans="1:26" ht="30" customHeight="1">
+    <row r="146" spans="1:26" ht="14">
       <c r="A146" s="7"/>
       <c r="B146" s="8"/>
       <c r="C146" s="9"/>
@@ -4668,7 +4668,7 @@
       <c r="Y147" s="6"/>
       <c r="Z147" s="6"/>
     </row>
-    <row r="148" spans="1:26" ht="30" customHeight="1">
+    <row r="148" spans="1:26" ht="14">
       <c r="A148" s="7"/>
       <c r="B148" s="8"/>
       <c r="C148" s="9"/>
@@ -4696,7 +4696,7 @@
       <c r="Y148" s="6"/>
       <c r="Z148" s="6"/>
     </row>
-    <row r="149" spans="1:26" ht="30" customHeight="1">
+    <row r="149" spans="1:26" ht="14">
       <c r="A149" s="7"/>
       <c r="B149" s="8"/>
       <c r="C149" s="9"/>
@@ -4752,7 +4752,7 @@
       <c r="Y150" s="6"/>
       <c r="Z150" s="6"/>
     </row>
-    <row r="151" spans="1:26" ht="30" customHeight="1">
+    <row r="151" spans="1:26" ht="14">
       <c r="A151" s="7"/>
       <c r="B151" s="8"/>
       <c r="C151" s="9"/>
@@ -4836,7 +4836,7 @@
       <c r="Y153" s="6"/>
       <c r="Z153" s="6"/>
     </row>
-    <row r="154" spans="1:26" ht="30" customHeight="1">
+    <row r="154" spans="1:26" ht="14">
       <c r="A154" s="7"/>
       <c r="B154" s="8"/>
       <c r="C154" s="9"/>
@@ -4920,7 +4920,7 @@
       <c r="Y156" s="6"/>
       <c r="Z156" s="6"/>
     </row>
-    <row r="157" spans="1:26" ht="30" customHeight="1">
+    <row r="157" spans="1:26" ht="14">
       <c r="A157" s="7"/>
       <c r="B157" s="8"/>
       <c r="C157" s="9"/>
@@ -5340,7 +5340,7 @@
       <c r="Y171" s="6"/>
       <c r="Z171" s="6"/>
     </row>
-    <row r="172" spans="1:26" ht="30" customHeight="1">
+    <row r="172" spans="1:26" ht="14">
       <c r="A172" s="12"/>
       <c r="B172" s="13"/>
       <c r="C172" s="14"/>
@@ -5368,7 +5368,7 @@
       <c r="Y172" s="6"/>
       <c r="Z172" s="6"/>
     </row>
-    <row r="173" spans="1:26" ht="30" customHeight="1">
+    <row r="173" spans="1:26" ht="14">
       <c r="A173" s="12"/>
       <c r="B173" s="13"/>
       <c r="C173" s="14"/>
@@ -5396,7 +5396,7 @@
       <c r="Y173" s="6"/>
       <c r="Z173" s="6"/>
     </row>
-    <row r="174" spans="1:26" ht="30" customHeight="1">
+    <row r="174" spans="1:26" ht="14">
       <c r="A174" s="12"/>
       <c r="B174" s="13"/>
       <c r="C174" s="14"/>
@@ -5676,7 +5676,7 @@
       <c r="Y183" s="6"/>
       <c r="Z183" s="6"/>
     </row>
-    <row r="184" spans="1:26" ht="30" customHeight="1">
+    <row r="184" spans="1:26" ht="14">
       <c r="A184" s="7"/>
       <c r="B184" s="8"/>
       <c r="C184" s="9"/>
@@ -5704,7 +5704,7 @@
       <c r="Y184" s="6"/>
       <c r="Z184" s="6"/>
     </row>
-    <row r="185" spans="1:26" ht="30" customHeight="1">
+    <row r="185" spans="1:26" ht="14">
       <c r="A185" s="7"/>
       <c r="B185" s="8"/>
       <c r="C185" s="9"/>
@@ -5732,7 +5732,7 @@
       <c r="Y185" s="6"/>
       <c r="Z185" s="6"/>
     </row>
-    <row r="186" spans="1:26" ht="30" customHeight="1">
+    <row r="186" spans="1:26" ht="14">
       <c r="A186" s="7"/>
       <c r="B186" s="8"/>
       <c r="C186" s="9"/>
@@ -5788,7 +5788,7 @@
       <c r="Y187" s="6"/>
       <c r="Z187" s="6"/>
     </row>
-    <row r="188" spans="1:26" ht="30" customHeight="1">
+    <row r="188" spans="1:26" ht="14">
       <c r="A188" s="7"/>
       <c r="B188" s="8"/>
       <c r="C188" s="9"/>
@@ -5816,7 +5816,7 @@
       <c r="Y188" s="6"/>
       <c r="Z188" s="6"/>
     </row>
-    <row r="189" spans="1:26" ht="60" customHeight="1">
+    <row r="189" spans="1:26" ht="14">
       <c r="A189" s="7"/>
       <c r="B189" s="8"/>
       <c r="C189" s="9"/>
@@ -5900,7 +5900,7 @@
       <c r="Y191" s="6"/>
       <c r="Z191" s="6"/>
     </row>
-    <row r="192" spans="1:26" ht="30" customHeight="1">
+    <row r="192" spans="1:26" ht="14">
       <c r="A192" s="7"/>
       <c r="B192" s="8"/>
       <c r="C192" s="9"/>
@@ -5928,7 +5928,7 @@
       <c r="Y192" s="6"/>
       <c r="Z192" s="6"/>
     </row>
-    <row r="193" spans="1:26" ht="30" customHeight="1">
+    <row r="193" spans="1:26" ht="14">
       <c r="A193" s="7"/>
       <c r="B193" s="8"/>
       <c r="C193" s="9"/>
@@ -6068,7 +6068,7 @@
       <c r="Y197" s="6"/>
       <c r="Z197" s="6"/>
     </row>
-    <row r="198" spans="1:26" ht="30" customHeight="1">
+    <row r="198" spans="1:26" ht="14">
       <c r="A198" s="12"/>
       <c r="B198" s="13"/>
       <c r="C198" s="14"/>
@@ -6124,7 +6124,7 @@
       <c r="Y199" s="6"/>
       <c r="Z199" s="6"/>
     </row>
-    <row r="200" spans="1:26" ht="30" customHeight="1">
+    <row r="200" spans="1:26" ht="14">
       <c r="A200" s="12"/>
       <c r="B200" s="13"/>
       <c r="C200" s="14"/>
@@ -6180,7 +6180,7 @@
       <c r="Y201" s="6"/>
       <c r="Z201" s="6"/>
     </row>
-    <row r="202" spans="1:26" ht="30" customHeight="1">
+    <row r="202" spans="1:26" ht="14">
       <c r="A202" s="12"/>
       <c r="B202" s="13"/>
       <c r="C202" s="14"/>
@@ -6348,7 +6348,7 @@
       <c r="Y207" s="6"/>
       <c r="Z207" s="6"/>
     </row>
-    <row r="208" spans="1:26" ht="30" customHeight="1">
+    <row r="208" spans="1:26" ht="14">
       <c r="A208" s="7"/>
       <c r="B208" s="8"/>
       <c r="C208" s="9"/>
@@ -6404,7 +6404,7 @@
       <c r="Y209" s="6"/>
       <c r="Z209" s="6"/>
     </row>
-    <row r="210" spans="1:26" ht="30" customHeight="1">
+    <row r="210" spans="1:26" ht="14">
       <c r="A210" s="7"/>
       <c r="B210" s="8"/>
       <c r="C210" s="9"/>
@@ -6460,7 +6460,7 @@
       <c r="Y211" s="6"/>
       <c r="Z211" s="6"/>
     </row>
-    <row r="212" spans="1:26" ht="30" customHeight="1">
+    <row r="212" spans="1:26" ht="14">
       <c r="A212" s="7"/>
       <c r="B212" s="8"/>
       <c r="C212" s="9"/>
@@ -6488,7 +6488,7 @@
       <c r="Y212" s="6"/>
       <c r="Z212" s="6"/>
     </row>
-    <row r="213" spans="1:26" ht="30" customHeight="1">
+    <row r="213" spans="1:26" ht="14">
       <c r="A213" s="7"/>
       <c r="B213" s="8"/>
       <c r="C213" s="9"/>
@@ -6656,7 +6656,7 @@
       <c r="Y218" s="6"/>
       <c r="Z218" s="6"/>
     </row>
-    <row r="219" spans="1:26" ht="30" customHeight="1">
+    <row r="219" spans="1:26" ht="14">
       <c r="A219" s="7"/>
       <c r="B219" s="8"/>
       <c r="C219" s="9"/>
@@ -6684,7 +6684,7 @@
       <c r="Y219" s="6"/>
       <c r="Z219" s="6"/>
     </row>
-    <row r="220" spans="1:26" ht="30" customHeight="1">
+    <row r="220" spans="1:26" ht="14">
       <c r="A220" s="7"/>
       <c r="B220" s="8"/>
       <c r="C220" s="9"/>
@@ -6740,7 +6740,7 @@
       <c r="Y221" s="6"/>
       <c r="Z221" s="6"/>
     </row>
-    <row r="222" spans="1:26" ht="30" customHeight="1">
+    <row r="222" spans="1:26" ht="14">
       <c r="A222" s="7"/>
       <c r="B222" s="8"/>
       <c r="C222" s="9"/>
@@ -6768,7 +6768,7 @@
       <c r="Y222" s="6"/>
       <c r="Z222" s="6"/>
     </row>
-    <row r="223" spans="1:26" ht="30" customHeight="1">
+    <row r="223" spans="1:26" ht="14">
       <c r="A223" s="7"/>
       <c r="B223" s="8"/>
       <c r="C223" s="9"/>
@@ -6880,7 +6880,7 @@
       <c r="Y226" s="6"/>
       <c r="Z226" s="6"/>
     </row>
-    <row r="227" spans="1:26" ht="30" customHeight="1">
+    <row r="227" spans="1:26" ht="14">
       <c r="A227" s="7"/>
       <c r="B227" s="8"/>
       <c r="C227" s="9"/>
@@ -6936,7 +6936,7 @@
       <c r="Y228" s="6"/>
       <c r="Z228" s="6"/>
     </row>
-    <row r="229" spans="1:26" ht="30" customHeight="1">
+    <row r="229" spans="1:26" ht="14">
       <c r="A229" s="7"/>
       <c r="B229" s="8"/>
       <c r="C229" s="9"/>
@@ -7020,7 +7020,7 @@
       <c r="Y231" s="6"/>
       <c r="Z231" s="6"/>
     </row>
-    <row r="232" spans="1:26" ht="30" customHeight="1">
+    <row r="232" spans="1:26" ht="14">
       <c r="A232" s="7"/>
       <c r="B232" s="8"/>
       <c r="C232" s="9"/>
@@ -7244,7 +7244,7 @@
       <c r="Y239" s="6"/>
       <c r="Z239" s="6"/>
     </row>
-    <row r="240" spans="1:26" ht="30" customHeight="1">
+    <row r="240" spans="1:26" ht="14">
       <c r="A240" s="12"/>
       <c r="B240" s="13"/>
       <c r="C240" s="14"/>
@@ -7440,7 +7440,7 @@
       <c r="Y246" s="6"/>
       <c r="Z246" s="6"/>
     </row>
-    <row r="247" spans="1:26" ht="30" customHeight="1">
+    <row r="247" spans="1:26" ht="14">
       <c r="A247" s="12"/>
       <c r="B247" s="13"/>
       <c r="C247" s="14"/>
@@ -7832,7 +7832,7 @@
       <c r="Y260" s="6"/>
       <c r="Z260" s="6"/>
     </row>
-    <row r="261" spans="1:26" ht="30" customHeight="1">
+    <row r="261" spans="1:26" ht="14">
       <c r="A261" s="7"/>
       <c r="B261" s="8"/>
       <c r="C261" s="9"/>
@@ -7944,7 +7944,7 @@
       <c r="Y264" s="6"/>
       <c r="Z264" s="6"/>
     </row>
-    <row r="265" spans="1:26" ht="30" customHeight="1">
+    <row r="265" spans="1:26" ht="14">
       <c r="A265" s="7"/>
       <c r="B265" s="8"/>
       <c r="C265" s="9"/>
@@ -8252,7 +8252,7 @@
       <c r="Y275" s="6"/>
       <c r="Z275" s="6"/>
     </row>
-    <row r="276" spans="1:26" ht="30" customHeight="1">
+    <row r="276" spans="1:26" ht="14">
       <c r="A276" s="7"/>
       <c r="B276" s="8"/>
       <c r="C276" s="9"/>
@@ -8364,7 +8364,7 @@
       <c r="Y279" s="6"/>
       <c r="Z279" s="6"/>
     </row>
-    <row r="280" spans="1:26" ht="30" customHeight="1">
+    <row r="280" spans="1:26" ht="14">
       <c r="A280" s="7"/>
       <c r="B280" s="8"/>
       <c r="C280" s="9"/>
@@ -8644,7 +8644,7 @@
       <c r="Y289" s="6"/>
       <c r="Z289" s="6"/>
     </row>
-    <row r="290" spans="1:26" ht="30" customHeight="1">
+    <row r="290" spans="1:26" ht="14">
       <c r="A290" s="7"/>
       <c r="B290" s="8"/>
       <c r="C290" s="9"/>
@@ -9176,7 +9176,7 @@
       <c r="Y308" s="6"/>
       <c r="Z308" s="6"/>
     </row>
-    <row r="309" spans="1:26" ht="30" customHeight="1">
+    <row r="309" spans="1:26" ht="14">
       <c r="A309" s="12"/>
       <c r="B309" s="13"/>
       <c r="C309" s="14"/>
@@ -9232,7 +9232,7 @@
       <c r="Y310" s="6"/>
       <c r="Z310" s="6"/>
     </row>
-    <row r="311" spans="1:26" ht="30" customHeight="1">
+    <row r="311" spans="1:26" ht="14">
       <c r="A311" s="12"/>
       <c r="B311" s="13"/>
       <c r="C311" s="14"/>
@@ -9372,7 +9372,7 @@
       <c r="Y315" s="6"/>
       <c r="Z315" s="6"/>
     </row>
-    <row r="316" spans="1:26" ht="30" customHeight="1">
+    <row r="316" spans="1:26" ht="14">
       <c r="A316" s="7"/>
       <c r="B316" s="8"/>
       <c r="C316" s="9"/>
@@ -9456,7 +9456,7 @@
       <c r="Y318" s="6"/>
       <c r="Z318" s="6"/>
     </row>
-    <row r="319" spans="1:26" ht="30" customHeight="1">
+    <row r="319" spans="1:26" ht="14">
       <c r="A319" s="7"/>
       <c r="B319" s="8"/>
       <c r="C319" s="9"/>
@@ -9736,7 +9736,7 @@
       <c r="Y328" s="6"/>
       <c r="Z328" s="6"/>
     </row>
-    <row r="329" spans="1:26" ht="30" customHeight="1">
+    <row r="329" spans="1:26" ht="14">
       <c r="A329" s="7"/>
       <c r="B329" s="8"/>
       <c r="C329" s="9"/>
@@ -9764,7 +9764,7 @@
       <c r="Y329" s="6"/>
       <c r="Z329" s="6"/>
     </row>
-    <row r="330" spans="1:26" ht="30" customHeight="1">
+    <row r="330" spans="1:26" ht="14">
       <c r="A330" s="7"/>
       <c r="B330" s="8"/>
       <c r="C330" s="9"/>
@@ -9820,7 +9820,7 @@
       <c r="Y331" s="6"/>
       <c r="Z331" s="6"/>
     </row>
-    <row r="332" spans="1:26" ht="30" customHeight="1">
+    <row r="332" spans="1:26" ht="14">
       <c r="A332" s="7"/>
       <c r="B332" s="8"/>
       <c r="C332" s="9"/>
@@ -9848,7 +9848,7 @@
       <c r="Y332" s="6"/>
       <c r="Z332" s="6"/>
     </row>
-    <row r="333" spans="1:26" ht="30" customHeight="1">
+    <row r="333" spans="1:26" ht="14">
       <c r="A333" s="7"/>
       <c r="B333" s="8"/>
       <c r="C333" s="9"/>
@@ -9904,7 +9904,7 @@
       <c r="Y334" s="6"/>
       <c r="Z334" s="6"/>
     </row>
-    <row r="335" spans="1:26" ht="30" customHeight="1">
+    <row r="335" spans="1:26" ht="14">
       <c r="A335" s="7"/>
       <c r="B335" s="8"/>
       <c r="C335" s="9"/>
@@ -9932,7 +9932,7 @@
       <c r="Y335" s="6"/>
       <c r="Z335" s="6"/>
     </row>
-    <row r="336" spans="1:26" ht="30" customHeight="1">
+    <row r="336" spans="1:26" ht="14">
       <c r="A336" s="7"/>
       <c r="B336" s="8"/>
       <c r="C336" s="9"/>
@@ -9960,7 +9960,7 @@
       <c r="Y336" s="6"/>
       <c r="Z336" s="6"/>
     </row>
-    <row r="337" spans="1:26" ht="30" customHeight="1">
+    <row r="337" spans="1:26" ht="14">
       <c r="A337" s="7"/>
       <c r="B337" s="8"/>
       <c r="C337" s="9"/>
@@ -9988,7 +9988,7 @@
       <c r="Y337" s="6"/>
       <c r="Z337" s="6"/>
     </row>
-    <row r="338" spans="1:26" ht="30" customHeight="1">
+    <row r="338" spans="1:26" ht="14">
       <c r="A338" s="7"/>
       <c r="B338" s="8"/>
       <c r="C338" s="9"/>
@@ -10016,7 +10016,7 @@
       <c r="Y338" s="6"/>
       <c r="Z338" s="6"/>
     </row>
-    <row r="339" spans="1:26" ht="30" customHeight="1">
+    <row r="339" spans="1:26" ht="14">
       <c r="A339" s="7"/>
       <c r="B339" s="8"/>
       <c r="C339" s="9"/>
@@ -10044,7 +10044,7 @@
       <c r="Y339" s="6"/>
       <c r="Z339" s="6"/>
     </row>
-    <row r="340" spans="1:26" ht="30" customHeight="1">
+    <row r="340" spans="1:26" ht="14">
       <c r="A340" s="7"/>
       <c r="B340" s="8"/>
       <c r="C340" s="9"/>
@@ -10072,7 +10072,7 @@
       <c r="Y340" s="6"/>
       <c r="Z340" s="6"/>
     </row>
-    <row r="341" spans="1:26" ht="30" customHeight="1">
+    <row r="341" spans="1:26" ht="14">
       <c r="A341" s="7"/>
       <c r="B341" s="8"/>
       <c r="C341" s="9"/>
@@ -10100,7 +10100,7 @@
       <c r="Y341" s="6"/>
       <c r="Z341" s="6"/>
     </row>
-    <row r="342" spans="1:26" ht="30" customHeight="1">
+    <row r="342" spans="1:26" ht="14">
       <c r="A342" s="7"/>
       <c r="B342" s="8"/>
       <c r="C342" s="9"/>
@@ -10184,7 +10184,7 @@
       <c r="Y344" s="6"/>
       <c r="Z344" s="6"/>
     </row>
-    <row r="345" spans="1:26" ht="30" customHeight="1">
+    <row r="345" spans="1:26" ht="14">
       <c r="A345" s="7"/>
       <c r="B345" s="8"/>
       <c r="C345" s="9"/>
@@ -10212,7 +10212,7 @@
       <c r="Y345" s="6"/>
       <c r="Z345" s="6"/>
     </row>
-    <row r="346" spans="1:26" ht="30" customHeight="1">
+    <row r="346" spans="1:26" ht="14">
       <c r="A346" s="12"/>
       <c r="B346" s="13"/>
       <c r="C346" s="14"/>
@@ -10380,7 +10380,7 @@
       <c r="Y351" s="6"/>
       <c r="Z351" s="6"/>
     </row>
-    <row r="352" spans="1:26" ht="30" customHeight="1">
+    <row r="352" spans="1:26" ht="14">
       <c r="A352" s="12"/>
       <c r="B352" s="13"/>
       <c r="C352" s="14"/>
@@ -10436,7 +10436,7 @@
       <c r="Y353" s="6"/>
       <c r="Z353" s="6"/>
     </row>
-    <row r="354" spans="1:26" ht="30" customHeight="1">
+    <row r="354" spans="1:26" ht="14">
       <c r="A354" s="7"/>
       <c r="B354" s="8"/>
       <c r="C354" s="9"/>
@@ -10464,7 +10464,7 @@
       <c r="Y354" s="6"/>
       <c r="Z354" s="6"/>
     </row>
-    <row r="355" spans="1:26" ht="30" customHeight="1">
+    <row r="355" spans="1:26" ht="14">
       <c r="A355" s="7"/>
       <c r="B355" s="8"/>
       <c r="C355" s="9"/>
@@ -10492,7 +10492,7 @@
       <c r="Y355" s="6"/>
       <c r="Z355" s="6"/>
     </row>
-    <row r="356" spans="1:26" ht="30" customHeight="1">
+    <row r="356" spans="1:26" ht="14">
       <c r="A356" s="7"/>
       <c r="B356" s="8"/>
       <c r="C356" s="9"/>
@@ -10520,7 +10520,7 @@
       <c r="Y356" s="6"/>
       <c r="Z356" s="6"/>
     </row>
-    <row r="357" spans="1:26" ht="30" customHeight="1">
+    <row r="357" spans="1:26" ht="14">
       <c r="A357" s="7"/>
       <c r="B357" s="8"/>
       <c r="C357" s="9"/>
@@ -10548,7 +10548,7 @@
       <c r="Y357" s="6"/>
       <c r="Z357" s="6"/>
     </row>
-    <row r="358" spans="1:26" ht="30" customHeight="1">
+    <row r="358" spans="1:26" ht="14">
       <c r="A358" s="7"/>
       <c r="B358" s="8"/>
       <c r="C358" s="9"/>
@@ -10576,7 +10576,7 @@
       <c r="Y358" s="6"/>
       <c r="Z358" s="6"/>
     </row>
-    <row r="359" spans="1:26" ht="30" customHeight="1">
+    <row r="359" spans="1:26" ht="14">
       <c r="A359" s="7"/>
       <c r="B359" s="8"/>
       <c r="C359" s="9"/>
@@ -10660,7 +10660,7 @@
       <c r="Y361" s="6"/>
       <c r="Z361" s="6"/>
     </row>
-    <row r="362" spans="1:26" ht="30" customHeight="1">
+    <row r="362" spans="1:26" ht="14">
       <c r="A362" s="7"/>
       <c r="B362" s="8"/>
       <c r="C362" s="9"/>
@@ -10716,7 +10716,7 @@
       <c r="Y363" s="6"/>
       <c r="Z363" s="6"/>
     </row>
-    <row r="364" spans="1:26" ht="30" customHeight="1">
+    <row r="364" spans="1:26" ht="14">
       <c r="A364" s="7"/>
       <c r="B364" s="8"/>
       <c r="C364" s="9"/>
@@ -10744,7 +10744,7 @@
       <c r="Y364" s="6"/>
       <c r="Z364" s="6"/>
     </row>
-    <row r="365" spans="1:26" ht="30" customHeight="1">
+    <row r="365" spans="1:26" ht="14">
       <c r="A365" s="7"/>
       <c r="B365" s="8"/>
       <c r="C365" s="9"/>
@@ -10800,7 +10800,7 @@
       <c r="Y366" s="6"/>
       <c r="Z366" s="6"/>
     </row>
-    <row r="367" spans="1:26" ht="30" customHeight="1">
+    <row r="367" spans="1:26" ht="14">
       <c r="A367" s="7"/>
       <c r="B367" s="8"/>
       <c r="C367" s="9"/>
@@ -10828,7 +10828,7 @@
       <c r="Y367" s="6"/>
       <c r="Z367" s="6"/>
     </row>
-    <row r="368" spans="1:26" ht="30" customHeight="1">
+    <row r="368" spans="1:26" ht="14">
       <c r="A368" s="7"/>
       <c r="B368" s="8"/>
       <c r="C368" s="9"/>
@@ -10856,7 +10856,7 @@
       <c r="Y368" s="6"/>
       <c r="Z368" s="6"/>
     </row>
-    <row r="369" spans="1:26" ht="30" customHeight="1">
+    <row r="369" spans="1:26" ht="14">
       <c r="A369" s="7"/>
       <c r="B369" s="8"/>
       <c r="C369" s="9"/>
@@ -10912,7 +10912,7 @@
       <c r="Y370" s="6"/>
       <c r="Z370" s="6"/>
     </row>
-    <row r="371" spans="1:26" ht="30" customHeight="1">
+    <row r="371" spans="1:26" ht="14">
       <c r="A371" s="7"/>
       <c r="B371" s="8"/>
       <c r="C371" s="9"/>
@@ -10968,7 +10968,7 @@
       <c r="Y372" s="6"/>
       <c r="Z372" s="6"/>
     </row>
-    <row r="373" spans="1:26" ht="30" customHeight="1">
+    <row r="373" spans="1:26" ht="14">
       <c r="A373" s="7"/>
       <c r="B373" s="8"/>
       <c r="C373" s="9"/>
@@ -10996,7 +10996,7 @@
       <c r="Y373" s="6"/>
       <c r="Z373" s="6"/>
     </row>
-    <row r="374" spans="1:26" ht="30" customHeight="1">
+    <row r="374" spans="1:26" ht="14">
       <c r="A374" s="7"/>
       <c r="B374" s="8"/>
       <c r="C374" s="9"/>
@@ -11080,7 +11080,7 @@
       <c r="Y376" s="6"/>
       <c r="Z376" s="6"/>
     </row>
-    <row r="377" spans="1:26" ht="30" customHeight="1">
+    <row r="377" spans="1:26" ht="14">
       <c r="A377" s="7"/>
       <c r="B377" s="8"/>
       <c r="C377" s="9"/>
@@ -11108,7 +11108,7 @@
       <c r="Y377" s="6"/>
       <c r="Z377" s="6"/>
     </row>
-    <row r="378" spans="1:26" ht="30" customHeight="1">
+    <row r="378" spans="1:26" ht="14">
       <c r="A378" s="7"/>
       <c r="B378" s="8"/>
       <c r="C378" s="9"/>
@@ -11192,7 +11192,7 @@
       <c r="Y380" s="6"/>
       <c r="Z380" s="6"/>
     </row>
-    <row r="381" spans="1:26" ht="30" customHeight="1">
+    <row r="381" spans="1:26" ht="14">
       <c r="A381" s="12"/>
       <c r="B381" s="13"/>
       <c r="C381" s="14"/>
@@ -11220,7 +11220,7 @@
       <c r="Y381" s="6"/>
       <c r="Z381" s="6"/>
     </row>
-    <row r="382" spans="1:26" ht="30" customHeight="1">
+    <row r="382" spans="1:26" ht="14">
       <c r="A382" s="12"/>
       <c r="B382" s="13"/>
       <c r="C382" s="14"/>
@@ -11248,7 +11248,7 @@
       <c r="Y382" s="6"/>
       <c r="Z382" s="6"/>
     </row>
-    <row r="383" spans="1:26" ht="30" customHeight="1">
+    <row r="383" spans="1:26" ht="14">
       <c r="A383" s="12"/>
       <c r="B383" s="13"/>
       <c r="C383" s="14"/>
@@ -11276,7 +11276,7 @@
       <c r="Y383" s="6"/>
       <c r="Z383" s="6"/>
     </row>
-    <row r="384" spans="1:26" ht="30" customHeight="1">
+    <row r="384" spans="1:26" ht="14">
       <c r="A384" s="12"/>
       <c r="B384" s="13"/>
       <c r="C384" s="14"/>
@@ -11500,7 +11500,7 @@
       <c r="Y391" s="6"/>
       <c r="Z391" s="6"/>
     </row>
-    <row r="392" spans="1:26" ht="30" customHeight="1">
+    <row r="392" spans="1:26" ht="14">
       <c r="A392" s="7"/>
       <c r="B392" s="16"/>
       <c r="C392" s="9"/>
@@ -11556,7 +11556,7 @@
       <c r="Y393" s="6"/>
       <c r="Z393" s="6"/>
     </row>
-    <row r="394" spans="1:26" ht="30" customHeight="1">
+    <row r="394" spans="1:26" ht="14">
       <c r="A394" s="7"/>
       <c r="B394" s="16"/>
       <c r="C394" s="9"/>
@@ -11612,7 +11612,7 @@
       <c r="Y395" s="6"/>
       <c r="Z395" s="6"/>
     </row>
-    <row r="396" spans="1:26" ht="30" customHeight="1">
+    <row r="396" spans="1:26" ht="14">
       <c r="A396" s="7"/>
       <c r="B396" s="16"/>
       <c r="C396" s="9"/>
@@ -11640,7 +11640,7 @@
       <c r="Y396" s="6"/>
       <c r="Z396" s="6"/>
     </row>
-    <row r="397" spans="1:26" ht="30" customHeight="1">
+    <row r="397" spans="1:26" ht="14">
       <c r="A397" s="7"/>
       <c r="B397" s="8"/>
       <c r="C397" s="9"/>
@@ -11668,7 +11668,7 @@
       <c r="Y397" s="6"/>
       <c r="Z397" s="6"/>
     </row>
-    <row r="398" spans="1:26" ht="30" customHeight="1">
+    <row r="398" spans="1:26" ht="14">
       <c r="A398" s="7"/>
       <c r="B398" s="16"/>
       <c r="C398" s="9"/>
@@ -11752,7 +11752,7 @@
       <c r="Y400" s="6"/>
       <c r="Z400" s="6"/>
     </row>
-    <row r="401" spans="1:26" ht="60" customHeight="1">
+    <row r="401" spans="1:26" ht="14">
       <c r="A401" s="7"/>
       <c r="B401" s="8"/>
       <c r="C401" s="9"/>
@@ -11780,7 +11780,7 @@
       <c r="Y401" s="6"/>
       <c r="Z401" s="6"/>
     </row>
-    <row r="402" spans="1:26" ht="60" customHeight="1">
+    <row r="402" spans="1:26" ht="14">
       <c r="A402" s="7"/>
       <c r="B402" s="16"/>
       <c r="C402" s="9"/>
@@ -11836,7 +11836,7 @@
       <c r="Y403" s="6"/>
       <c r="Z403" s="6"/>
     </row>
-    <row r="404" spans="1:26" ht="30" customHeight="1">
+    <row r="404" spans="1:26" ht="14">
       <c r="A404" s="7"/>
       <c r="B404" s="16"/>
       <c r="C404" s="9"/>
@@ -11864,7 +11864,7 @@
       <c r="Y404" s="6"/>
       <c r="Z404" s="6"/>
     </row>
-    <row r="405" spans="1:26" ht="30" customHeight="1">
+    <row r="405" spans="1:26" ht="14">
       <c r="A405" s="7"/>
       <c r="B405" s="8"/>
       <c r="C405" s="9"/>
@@ -11892,7 +11892,7 @@
       <c r="Y405" s="6"/>
       <c r="Z405" s="6"/>
     </row>
-    <row r="406" spans="1:26" ht="30" customHeight="1">
+    <row r="406" spans="1:26" ht="14">
       <c r="A406" s="7"/>
       <c r="B406" s="16"/>
       <c r="C406" s="9"/>
@@ -11948,7 +11948,7 @@
       <c r="Y407" s="6"/>
       <c r="Z407" s="6"/>
     </row>
-    <row r="408" spans="1:26" ht="30" customHeight="1">
+    <row r="408" spans="1:26" ht="14">
       <c r="A408" s="7"/>
       <c r="B408" s="16"/>
       <c r="C408" s="9"/>
@@ -11976,7 +11976,7 @@
       <c r="Y408" s="6"/>
       <c r="Z408" s="6"/>
     </row>
-    <row r="409" spans="1:26" ht="30" customHeight="1">
+    <row r="409" spans="1:26" ht="14">
       <c r="A409" s="7"/>
       <c r="B409" s="8"/>
       <c r="C409" s="9"/>
@@ -12004,7 +12004,7 @@
       <c r="Y409" s="6"/>
       <c r="Z409" s="6"/>
     </row>
-    <row r="410" spans="1:26" ht="30" customHeight="1">
+    <row r="410" spans="1:26" ht="14">
       <c r="A410" s="7"/>
       <c r="B410" s="16"/>
       <c r="C410" s="9"/>
@@ -12032,7 +12032,7 @@
       <c r="Y410" s="6"/>
       <c r="Z410" s="6"/>
     </row>
-    <row r="411" spans="1:26" ht="30" customHeight="1">
+    <row r="411" spans="1:26" ht="14">
       <c r="A411" s="7"/>
       <c r="B411" s="8"/>
       <c r="C411" s="9"/>
@@ -12060,7 +12060,7 @@
       <c r="Y411" s="6"/>
       <c r="Z411" s="6"/>
     </row>
-    <row r="412" spans="1:26" ht="30" customHeight="1">
+    <row r="412" spans="1:26" ht="14">
       <c r="A412" s="7"/>
       <c r="B412" s="16"/>
       <c r="C412" s="9"/>
@@ -12088,7 +12088,7 @@
       <c r="Y412" s="6"/>
       <c r="Z412" s="6"/>
     </row>
-    <row r="413" spans="1:26" ht="30" customHeight="1">
+    <row r="413" spans="1:26" ht="14">
       <c r="A413" s="7"/>
       <c r="B413" s="8"/>
       <c r="C413" s="9"/>
@@ -12116,7 +12116,7 @@
       <c r="Y413" s="6"/>
       <c r="Z413" s="6"/>
     </row>
-    <row r="414" spans="1:26" ht="30" customHeight="1">
+    <row r="414" spans="1:26" ht="14">
       <c r="A414" s="7"/>
       <c r="B414" s="16"/>
       <c r="C414" s="9"/>
@@ -12144,7 +12144,7 @@
       <c r="Y414" s="6"/>
       <c r="Z414" s="6"/>
     </row>
-    <row r="415" spans="1:26" ht="30" customHeight="1">
+    <row r="415" spans="1:26" ht="14">
       <c r="A415" s="7"/>
       <c r="B415" s="8"/>
       <c r="C415" s="9"/>
@@ -12200,7 +12200,7 @@
       <c r="Y416" s="6"/>
       <c r="Z416" s="6"/>
     </row>
-    <row r="417" spans="1:26" ht="30" customHeight="1">
+    <row r="417" spans="1:26" ht="14">
       <c r="A417" s="7"/>
       <c r="B417" s="8"/>
       <c r="C417" s="9"/>
@@ -12228,7 +12228,7 @@
       <c r="Y417" s="6"/>
       <c r="Z417" s="6"/>
     </row>
-    <row r="418" spans="1:26" ht="30" customHeight="1">
+    <row r="418" spans="1:26" ht="14">
       <c r="A418" s="7"/>
       <c r="B418" s="16"/>
       <c r="C418" s="9"/>
@@ -12256,7 +12256,7 @@
       <c r="Y418" s="6"/>
       <c r="Z418" s="6"/>
     </row>
-    <row r="419" spans="1:26" ht="30" customHeight="1">
+    <row r="419" spans="1:26" ht="14">
       <c r="A419" s="7"/>
       <c r="B419" s="8"/>
       <c r="C419" s="9"/>
@@ -12284,7 +12284,7 @@
       <c r="Y419" s="6"/>
       <c r="Z419" s="6"/>
     </row>
-    <row r="420" spans="1:26" ht="30" customHeight="1">
+    <row r="420" spans="1:26" ht="14">
       <c r="A420" s="7"/>
       <c r="B420" s="16"/>
       <c r="C420" s="9"/>
@@ -12312,7 +12312,7 @@
       <c r="Y420" s="6"/>
       <c r="Z420" s="6"/>
     </row>
-    <row r="421" spans="1:26" ht="30" customHeight="1">
+    <row r="421" spans="1:26" ht="14">
       <c r="A421" s="7"/>
       <c r="B421" s="8"/>
       <c r="C421" s="9"/>
@@ -12368,7 +12368,7 @@
       <c r="Y422" s="6"/>
       <c r="Z422" s="6"/>
     </row>
-    <row r="423" spans="1:26" ht="30" customHeight="1">
+    <row r="423" spans="1:26" ht="14">
       <c r="A423" s="7"/>
       <c r="B423" s="8"/>
       <c r="C423" s="9"/>
@@ -12396,7 +12396,7 @@
       <c r="Y423" s="6"/>
       <c r="Z423" s="6"/>
     </row>
-    <row r="424" spans="1:26" ht="30" customHeight="1">
+    <row r="424" spans="1:26" ht="14">
       <c r="A424" s="7"/>
       <c r="B424" s="16"/>
       <c r="C424" s="9"/>
@@ -12424,7 +12424,7 @@
       <c r="Y424" s="6"/>
       <c r="Z424" s="6"/>
     </row>
-    <row r="425" spans="1:26" ht="30" customHeight="1">
+    <row r="425" spans="1:26" ht="14">
       <c r="A425" s="7"/>
       <c r="B425" s="8"/>
       <c r="C425" s="9"/>
@@ -12452,7 +12452,7 @@
       <c r="Y425" s="6"/>
       <c r="Z425" s="6"/>
     </row>
-    <row r="426" spans="1:26" ht="30" customHeight="1">
+    <row r="426" spans="1:26" ht="14">
       <c r="A426" s="7"/>
       <c r="B426" s="16"/>
       <c r="C426" s="9"/>
@@ -12508,7 +12508,7 @@
       <c r="Y427" s="6"/>
       <c r="Z427" s="6"/>
     </row>
-    <row r="428" spans="1:26" ht="30" customHeight="1">
+    <row r="428" spans="1:26" ht="14">
       <c r="A428" s="7"/>
       <c r="B428" s="16"/>
       <c r="C428" s="9"/>
@@ -12620,7 +12620,7 @@
       <c r="Y431" s="6"/>
       <c r="Z431" s="6"/>
     </row>
-    <row r="432" spans="1:26" ht="30" customHeight="1">
+    <row r="432" spans="1:26" ht="14">
       <c r="A432" s="7"/>
       <c r="B432" s="16"/>
       <c r="C432" s="9"/>
@@ -12648,7 +12648,7 @@
       <c r="Y432" s="6"/>
       <c r="Z432" s="6"/>
     </row>
-    <row r="433" spans="1:26" ht="30" customHeight="1">
+    <row r="433" spans="1:26" ht="14">
       <c r="A433" s="7"/>
       <c r="B433" s="8"/>
       <c r="C433" s="9"/>
@@ -12676,7 +12676,7 @@
       <c r="Y433" s="6"/>
       <c r="Z433" s="6"/>
     </row>
-    <row r="434" spans="1:26" ht="30" customHeight="1">
+    <row r="434" spans="1:26" ht="14">
       <c r="A434" s="7"/>
       <c r="B434" s="16"/>
       <c r="C434" s="9"/>
@@ -12704,7 +12704,7 @@
       <c r="Y434" s="6"/>
       <c r="Z434" s="6"/>
     </row>
-    <row r="435" spans="1:26" ht="30" customHeight="1">
+    <row r="435" spans="1:26" ht="14">
       <c r="A435" s="7"/>
       <c r="B435" s="8"/>
       <c r="C435" s="9"/>
@@ -12816,7 +12816,7 @@
       <c r="Y438" s="6"/>
       <c r="Z438" s="6"/>
     </row>
-    <row r="439" spans="1:26" ht="30" customHeight="1">
+    <row r="439" spans="1:26" ht="14">
       <c r="A439" s="7"/>
       <c r="B439" s="8"/>
       <c r="C439" s="9"/>
@@ -12844,7 +12844,7 @@
       <c r="Y439" s="6"/>
       <c r="Z439" s="6"/>
     </row>
-    <row r="440" spans="1:26" ht="30" customHeight="1">
+    <row r="440" spans="1:26" ht="14">
       <c r="A440" s="7"/>
       <c r="B440" s="16"/>
       <c r="C440" s="9"/>
@@ -12872,7 +12872,7 @@
       <c r="Y440" s="6"/>
       <c r="Z440" s="6"/>
     </row>
-    <row r="441" spans="1:26" ht="30" customHeight="1">
+    <row r="441" spans="1:26" ht="14">
       <c r="A441" s="7"/>
       <c r="B441" s="8"/>
       <c r="C441" s="9"/>
@@ -12900,7 +12900,7 @@
       <c r="Y441" s="6"/>
       <c r="Z441" s="6"/>
     </row>
-    <row r="442" spans="1:26" ht="30" customHeight="1">
+    <row r="442" spans="1:26" ht="14">
       <c r="A442" s="7"/>
       <c r="B442" s="16"/>
       <c r="C442" s="9"/>
@@ -12928,7 +12928,7 @@
       <c r="Y442" s="6"/>
       <c r="Z442" s="6"/>
     </row>
-    <row r="443" spans="1:26" ht="30" customHeight="1">
+    <row r="443" spans="1:26" ht="14">
       <c r="A443" s="7"/>
       <c r="B443" s="8"/>
       <c r="C443" s="9"/>
@@ -12956,7 +12956,7 @@
       <c r="Y443" s="6"/>
       <c r="Z443" s="6"/>
     </row>
-    <row r="444" spans="1:26" ht="30" customHeight="1">
+    <row r="444" spans="1:26" ht="14">
       <c r="A444" s="7"/>
       <c r="B444" s="16"/>
       <c r="C444" s="9"/>
@@ -13068,7 +13068,7 @@
       <c r="Y447" s="6"/>
       <c r="Z447" s="6"/>
     </row>
-    <row r="448" spans="1:26" ht="30" customHeight="1">
+    <row r="448" spans="1:26" ht="14">
       <c r="A448" s="7"/>
       <c r="B448" s="16"/>
       <c r="C448" s="9"/>
@@ -13124,7 +13124,7 @@
       <c r="Y449" s="6"/>
       <c r="Z449" s="6"/>
     </row>
-    <row r="450" spans="1:26" ht="30" customHeight="1">
+    <row r="450" spans="1:26" ht="14">
       <c r="A450" s="7"/>
       <c r="B450" s="16"/>
       <c r="C450" s="9"/>
@@ -13152,7 +13152,7 @@
       <c r="Y450" s="6"/>
       <c r="Z450" s="6"/>
     </row>
-    <row r="451" spans="1:26" ht="30" customHeight="1">
+    <row r="451" spans="1:26" ht="14">
       <c r="A451" s="7"/>
       <c r="B451" s="8"/>
       <c r="C451" s="9"/>
@@ -13180,7 +13180,7 @@
       <c r="Y451" s="6"/>
       <c r="Z451" s="6"/>
     </row>
-    <row r="452" spans="1:26" ht="30" customHeight="1">
+    <row r="452" spans="1:26" ht="14">
       <c r="A452" s="7"/>
       <c r="B452" s="16"/>
       <c r="C452" s="9"/>
@@ -13208,7 +13208,7 @@
       <c r="Y452" s="6"/>
       <c r="Z452" s="6"/>
     </row>
-    <row r="453" spans="1:26" ht="30" customHeight="1">
+    <row r="453" spans="1:26" ht="14">
       <c r="A453" s="7"/>
       <c r="B453" s="8"/>
       <c r="C453" s="9"/>
@@ -13236,7 +13236,7 @@
       <c r="Y453" s="6"/>
       <c r="Z453" s="6"/>
     </row>
-    <row r="454" spans="1:26" ht="30" customHeight="1">
+    <row r="454" spans="1:26" ht="14">
       <c r="A454" s="7"/>
       <c r="B454" s="16"/>
       <c r="C454" s="9"/>
@@ -13264,7 +13264,7 @@
       <c r="Y454" s="6"/>
       <c r="Z454" s="6"/>
     </row>
-    <row r="455" spans="1:26" ht="30" customHeight="1">
+    <row r="455" spans="1:26" ht="14">
       <c r="A455" s="7"/>
       <c r="B455" s="8"/>
       <c r="C455" s="9"/>
@@ -13292,7 +13292,7 @@
       <c r="Y455" s="6"/>
       <c r="Z455" s="6"/>
     </row>
-    <row r="456" spans="1:26" ht="30" customHeight="1">
+    <row r="456" spans="1:26" ht="14">
       <c r="A456" s="7"/>
       <c r="B456" s="16"/>
       <c r="C456" s="9"/>
@@ -13320,7 +13320,7 @@
       <c r="Y456" s="6"/>
       <c r="Z456" s="6"/>
     </row>
-    <row r="457" spans="1:26" ht="30" customHeight="1">
+    <row r="457" spans="1:26" ht="14">
       <c r="A457" s="7"/>
       <c r="B457" s="16"/>
       <c r="C457" s="9"/>
@@ -13684,7 +13684,7 @@
       <c r="Y469" s="6"/>
       <c r="Z469" s="6"/>
     </row>
-    <row r="470" spans="1:26" ht="30" customHeight="1">
+    <row r="470" spans="1:26" ht="14">
       <c r="A470" s="12"/>
       <c r="B470" s="13"/>
       <c r="C470" s="14"/>
@@ -14020,7 +14020,7 @@
       <c r="Y481" s="6"/>
       <c r="Z481" s="6"/>
     </row>
-    <row r="482" spans="1:26" ht="30" customHeight="1">
+    <row r="482" spans="1:26" ht="14">
       <c r="A482" s="12"/>
       <c r="B482" s="13"/>
       <c r="C482" s="14"/>
@@ -14104,7 +14104,7 @@
       <c r="Y484" s="6"/>
       <c r="Z484" s="6"/>
     </row>
-    <row r="485" spans="1:26" ht="30" customHeight="1">
+    <row r="485" spans="1:26" ht="14">
       <c r="A485" s="12"/>
       <c r="B485" s="13"/>
       <c r="C485" s="14"/>
@@ -14132,7 +14132,7 @@
       <c r="Y485" s="6"/>
       <c r="Z485" s="6"/>
     </row>
-    <row r="486" spans="1:26" ht="30" customHeight="1">
+    <row r="486" spans="1:26" ht="14">
       <c r="A486" s="12"/>
       <c r="B486" s="13"/>
       <c r="C486" s="14"/>
@@ -14216,7 +14216,7 @@
       <c r="Y488" s="6"/>
       <c r="Z488" s="6"/>
     </row>
-    <row r="489" spans="1:26" ht="30" customHeight="1">
+    <row r="489" spans="1:26" ht="14">
       <c r="A489" s="12"/>
       <c r="B489" s="13"/>
       <c r="C489" s="14"/>
@@ -14244,7 +14244,7 @@
       <c r="Y489" s="6"/>
       <c r="Z489" s="6"/>
     </row>
-    <row r="490" spans="1:26" ht="30" customHeight="1">
+    <row r="490" spans="1:26" ht="14">
       <c r="A490" s="12"/>
       <c r="B490" s="13"/>
       <c r="C490" s="14"/>
@@ -14272,7 +14272,7 @@
       <c r="Y490" s="6"/>
       <c r="Z490" s="6"/>
     </row>
-    <row r="491" spans="1:26" ht="30" customHeight="1">
+    <row r="491" spans="1:26" ht="14">
       <c r="A491" s="7"/>
       <c r="B491" s="16"/>
       <c r="C491" s="9"/>
@@ -14300,7 +14300,7 @@
       <c r="Y491" s="6"/>
       <c r="Z491" s="6"/>
     </row>
-    <row r="492" spans="1:26" ht="30" customHeight="1">
+    <row r="492" spans="1:26" ht="14">
       <c r="A492" s="7"/>
       <c r="B492" s="16"/>
       <c r="C492" s="9"/>
@@ -14328,7 +14328,7 @@
       <c r="Y492" s="6"/>
       <c r="Z492" s="6"/>
     </row>
-    <row r="493" spans="1:26" ht="30" customHeight="1">
+    <row r="493" spans="1:26" ht="14">
       <c r="A493" s="7"/>
       <c r="B493" s="16"/>
       <c r="C493" s="9"/>
@@ -14384,7 +14384,7 @@
       <c r="Y494" s="6"/>
       <c r="Z494" s="6"/>
     </row>
-    <row r="495" spans="1:26" ht="30" customHeight="1">
+    <row r="495" spans="1:26" ht="14">
       <c r="A495" s="7"/>
       <c r="B495" s="16"/>
       <c r="C495" s="9"/>
@@ -14412,7 +14412,7 @@
       <c r="Y495" s="6"/>
       <c r="Z495" s="6"/>
     </row>
-    <row r="496" spans="1:26" ht="30" customHeight="1">
+    <row r="496" spans="1:26" ht="14">
       <c r="A496" s="7"/>
       <c r="B496" s="16"/>
       <c r="C496" s="9"/>
@@ -14440,7 +14440,7 @@
       <c r="Y496" s="6"/>
       <c r="Z496" s="6"/>
     </row>
-    <row r="497" spans="1:26" ht="30" customHeight="1">
+    <row r="497" spans="1:26" ht="14">
       <c r="A497" s="7"/>
       <c r="B497" s="16"/>
       <c r="C497" s="9"/>
@@ -14496,7 +14496,7 @@
       <c r="Y498" s="6"/>
       <c r="Z498" s="6"/>
     </row>
-    <row r="499" spans="1:26" ht="30" customHeight="1">
+    <row r="499" spans="1:26" ht="14">
       <c r="A499" s="7"/>
       <c r="B499" s="16"/>
       <c r="C499" s="9"/>
@@ -14524,7 +14524,7 @@
       <c r="Y499" s="6"/>
       <c r="Z499" s="6"/>
     </row>
-    <row r="500" spans="1:26" ht="30" customHeight="1">
+    <row r="500" spans="1:26" ht="14">
       <c r="A500" s="7"/>
       <c r="B500" s="16"/>
       <c r="C500" s="9"/>
@@ -14552,7 +14552,7 @@
       <c r="Y500" s="6"/>
       <c r="Z500" s="6"/>
     </row>
-    <row r="501" spans="1:26" ht="30" customHeight="1">
+    <row r="501" spans="1:26" ht="14">
       <c r="A501" s="7"/>
       <c r="B501" s="16"/>
       <c r="C501" s="9"/>
@@ -14580,7 +14580,7 @@
       <c r="Y501" s="6"/>
       <c r="Z501" s="6"/>
     </row>
-    <row r="502" spans="1:26" ht="30" customHeight="1">
+    <row r="502" spans="1:26" ht="14">
       <c r="A502" s="7"/>
       <c r="B502" s="16"/>
       <c r="C502" s="9"/>
@@ -14720,7 +14720,7 @@
       <c r="Y506" s="6"/>
       <c r="Z506" s="6"/>
     </row>
-    <row r="507" spans="1:26" ht="30" customHeight="1">
+    <row r="507" spans="1:26" ht="14">
       <c r="A507" s="7"/>
       <c r="B507" s="16"/>
       <c r="C507" s="9"/>
@@ -14804,7 +14804,7 @@
       <c r="Y509" s="6"/>
       <c r="Z509" s="6"/>
     </row>
-    <row r="510" spans="1:26" ht="30" customHeight="1">
+    <row r="510" spans="1:26" ht="14">
       <c r="A510" s="7"/>
       <c r="B510" s="16"/>
       <c r="C510" s="9"/>
@@ -14832,7 +14832,7 @@
       <c r="Y510" s="6"/>
       <c r="Z510" s="6"/>
     </row>
-    <row r="511" spans="1:26" ht="30" customHeight="1">
+    <row r="511" spans="1:26" ht="14">
       <c r="A511" s="7"/>
       <c r="B511" s="16"/>
       <c r="C511" s="9"/>
@@ -14888,7 +14888,7 @@
       <c r="Y512" s="6"/>
       <c r="Z512" s="6"/>
     </row>
-    <row r="513" spans="1:26" ht="30" customHeight="1">
+    <row r="513" spans="1:26" ht="14">
       <c r="A513" s="7"/>
       <c r="B513" s="16"/>
       <c r="C513" s="9"/>
@@ -14944,7 +14944,7 @@
       <c r="Y514" s="6"/>
       <c r="Z514" s="6"/>
     </row>
-    <row r="515" spans="1:26" ht="30" customHeight="1">
+    <row r="515" spans="1:26" ht="14">
       <c r="A515" s="7"/>
       <c r="B515" s="16"/>
       <c r="C515" s="9"/>
@@ -14972,7 +14972,7 @@
       <c r="Y515" s="6"/>
       <c r="Z515" s="6"/>
     </row>
-    <row r="516" spans="1:26" ht="30" customHeight="1">
+    <row r="516" spans="1:26" ht="14">
       <c r="A516" s="7"/>
       <c r="B516" s="16"/>
       <c r="C516" s="9"/>
@@ -15056,7 +15056,7 @@
       <c r="Y518" s="6"/>
       <c r="Z518" s="6"/>
     </row>
-    <row r="519" spans="1:26" ht="30" customHeight="1">
+    <row r="519" spans="1:26" ht="14">
       <c r="A519" s="7"/>
       <c r="B519" s="16"/>
       <c r="C519" s="9"/>
@@ -15084,7 +15084,7 @@
       <c r="Y519" s="6"/>
       <c r="Z519" s="6"/>
     </row>
-    <row r="520" spans="1:26" ht="30" customHeight="1">
+    <row r="520" spans="1:26" ht="14">
       <c r="A520" s="7"/>
       <c r="B520" s="16"/>
       <c r="C520" s="9"/>
@@ -15168,7 +15168,7 @@
       <c r="Y522" s="6"/>
       <c r="Z522" s="6"/>
     </row>
-    <row r="523" spans="1:26" ht="30" customHeight="1">
+    <row r="523" spans="1:26" ht="14">
       <c r="A523" s="7"/>
       <c r="B523" s="8"/>
       <c r="C523" s="9"/>
@@ -15252,7 +15252,7 @@
       <c r="Y525" s="6"/>
       <c r="Z525" s="6"/>
     </row>
-    <row r="526" spans="1:26" ht="30" customHeight="1">
+    <row r="526" spans="1:26" ht="14">
       <c r="A526" s="7"/>
       <c r="B526" s="8"/>
       <c r="C526" s="9"/>
@@ -15280,7 +15280,7 @@
       <c r="Y526" s="6"/>
       <c r="Z526" s="6"/>
     </row>
-    <row r="527" spans="1:26" ht="30" customHeight="1">
+    <row r="527" spans="1:26" ht="14">
       <c r="A527" s="7"/>
       <c r="B527" s="8"/>
       <c r="C527" s="9"/>
@@ -15308,7 +15308,7 @@
       <c r="Y527" s="6"/>
       <c r="Z527" s="6"/>
     </row>
-    <row r="528" spans="1:26" ht="30" customHeight="1">
+    <row r="528" spans="1:26" ht="14">
       <c r="A528" s="12"/>
       <c r="B528" s="13"/>
       <c r="C528" s="14"/>
@@ -15448,7 +15448,7 @@
       <c r="Y532" s="6"/>
       <c r="Z532" s="6"/>
     </row>
-    <row r="533" spans="1:26" ht="30" customHeight="1">
+    <row r="533" spans="1:26" ht="14">
       <c r="A533" s="12"/>
       <c r="B533" s="13"/>
       <c r="C533" s="14"/>
@@ -15532,7 +15532,7 @@
       <c r="Y535" s="6"/>
       <c r="Z535" s="6"/>
     </row>
-    <row r="536" spans="1:26" ht="30" customHeight="1">
+    <row r="536" spans="1:26" ht="14">
       <c r="A536" s="12"/>
       <c r="B536" s="13"/>
       <c r="C536" s="14"/>
@@ -15728,7 +15728,7 @@
       <c r="Y542" s="6"/>
       <c r="Z542" s="6"/>
     </row>
-    <row r="543" spans="1:26" ht="30" customHeight="1">
+    <row r="543" spans="1:26" ht="14">
       <c r="A543" s="12"/>
       <c r="B543" s="13"/>
       <c r="C543" s="14"/>
@@ -15784,7 +15784,7 @@
       <c r="Y544" s="6"/>
       <c r="Z544" s="6"/>
     </row>
-    <row r="545" spans="1:26" ht="30" customHeight="1">
+    <row r="545" spans="1:26" ht="14">
       <c r="A545" s="12"/>
       <c r="B545" s="13"/>
       <c r="C545" s="14"/>
@@ -15812,7 +15812,7 @@
       <c r="Y545" s="6"/>
       <c r="Z545" s="6"/>
     </row>
-    <row r="546" spans="1:26" ht="30" customHeight="1">
+    <row r="546" spans="1:26" ht="14">
       <c r="A546" s="7"/>
       <c r="B546" s="16"/>
       <c r="C546" s="9"/>
@@ -15840,7 +15840,7 @@
       <c r="Y546" s="6"/>
       <c r="Z546" s="6"/>
     </row>
-    <row r="547" spans="1:26" ht="30" customHeight="1">
+    <row r="547" spans="1:26" ht="14">
       <c r="A547" s="7"/>
       <c r="B547" s="16"/>
       <c r="C547" s="9"/>
@@ -15896,7 +15896,7 @@
       <c r="Y548" s="6"/>
       <c r="Z548" s="6"/>
     </row>
-    <row r="549" spans="1:26" ht="30" customHeight="1">
+    <row r="549" spans="1:26" ht="14">
       <c r="A549" s="7"/>
       <c r="B549" s="16"/>
       <c r="C549" s="9"/>
@@ -15924,7 +15924,7 @@
       <c r="Y549" s="6"/>
       <c r="Z549" s="6"/>
     </row>
-    <row r="550" spans="1:26" ht="30" customHeight="1">
+    <row r="550" spans="1:26" ht="14">
       <c r="A550" s="7"/>
       <c r="B550" s="16"/>
       <c r="C550" s="9"/>
@@ -15980,7 +15980,7 @@
       <c r="Y551" s="6"/>
       <c r="Z551" s="6"/>
     </row>
-    <row r="552" spans="1:26" ht="30" customHeight="1">
+    <row r="552" spans="1:26" ht="14">
       <c r="A552" s="7"/>
       <c r="B552" s="16"/>
       <c r="C552" s="9"/>
@@ -16008,7 +16008,7 @@
       <c r="Y552" s="6"/>
       <c r="Z552" s="6"/>
     </row>
-    <row r="553" spans="1:26" ht="30" customHeight="1">
+    <row r="553" spans="1:26" ht="14">
       <c r="A553" s="7"/>
       <c r="B553" s="16"/>
       <c r="C553" s="9"/>
@@ -16064,7 +16064,7 @@
       <c r="Y554" s="6"/>
       <c r="Z554" s="6"/>
     </row>
-    <row r="555" spans="1:26" ht="30" customHeight="1">
+    <row r="555" spans="1:26" ht="14">
       <c r="A555" s="7"/>
       <c r="B555" s="16"/>
       <c r="C555" s="9"/>
@@ -16148,7 +16148,7 @@
       <c r="Y557" s="6"/>
       <c r="Z557" s="6"/>
     </row>
-    <row r="558" spans="1:26" ht="30" customHeight="1">
+    <row r="558" spans="1:26" ht="14">
       <c r="A558" s="7"/>
       <c r="B558" s="16"/>
       <c r="C558" s="9"/>
@@ -16204,7 +16204,7 @@
       <c r="Y559" s="6"/>
       <c r="Z559" s="6"/>
     </row>
-    <row r="560" spans="1:26" ht="30" customHeight="1">
+    <row r="560" spans="1:26" ht="14">
       <c r="A560" s="7"/>
       <c r="B560" s="16"/>
       <c r="C560" s="9"/>
@@ -16232,7 +16232,7 @@
       <c r="Y560" s="6"/>
       <c r="Z560" s="6"/>
     </row>
-    <row r="561" spans="1:26" ht="30" customHeight="1">
+    <row r="561" spans="1:26" ht="14">
       <c r="A561" s="7"/>
       <c r="B561" s="16"/>
       <c r="C561" s="9"/>
@@ -16288,7 +16288,7 @@
       <c r="Y562" s="6"/>
       <c r="Z562" s="6"/>
     </row>
-    <row r="563" spans="1:26" ht="30" customHeight="1">
+    <row r="563" spans="1:26" ht="14">
       <c r="A563" s="7"/>
       <c r="B563" s="16"/>
       <c r="C563" s="9"/>
@@ -16316,7 +16316,7 @@
       <c r="Y563" s="6"/>
       <c r="Z563" s="6"/>
     </row>
-    <row r="564" spans="1:26" ht="30" customHeight="1">
+    <row r="564" spans="1:26" ht="14">
       <c r="A564" s="7"/>
       <c r="B564" s="16"/>
       <c r="C564" s="9"/>
@@ -16344,7 +16344,7 @@
       <c r="Y564" s="6"/>
       <c r="Z564" s="6"/>
     </row>
-    <row r="565" spans="1:26" ht="30" customHeight="1">
+    <row r="565" spans="1:26" ht="14">
       <c r="A565" s="7"/>
       <c r="B565" s="16"/>
       <c r="C565" s="9"/>
@@ -16372,7 +16372,7 @@
       <c r="Y565" s="6"/>
       <c r="Z565" s="6"/>
     </row>
-    <row r="566" spans="1:26" ht="30" customHeight="1">
+    <row r="566" spans="1:26" ht="14">
       <c r="A566" s="7"/>
       <c r="B566" s="16"/>
       <c r="C566" s="9"/>
@@ -16428,7 +16428,7 @@
       <c r="Y567" s="6"/>
       <c r="Z567" s="6"/>
     </row>
-    <row r="568" spans="1:26" ht="30" customHeight="1">
+    <row r="568" spans="1:26" ht="14">
       <c r="A568" s="7"/>
       <c r="B568" s="16"/>
       <c r="C568" s="9"/>
@@ -16456,7 +16456,7 @@
       <c r="Y568" s="6"/>
       <c r="Z568" s="6"/>
     </row>
-    <row r="569" spans="1:26" ht="30" customHeight="1">
+    <row r="569" spans="1:26" ht="14">
       <c r="A569" s="7"/>
       <c r="B569" s="16"/>
       <c r="C569" s="9"/>
@@ -16484,7 +16484,7 @@
       <c r="Y569" s="6"/>
       <c r="Z569" s="6"/>
     </row>
-    <row r="570" spans="1:26" ht="30" customHeight="1">
+    <row r="570" spans="1:26" ht="14">
       <c r="A570" s="7"/>
       <c r="B570" s="16"/>
       <c r="C570" s="9"/>
@@ -16512,7 +16512,7 @@
       <c r="Y570" s="6"/>
       <c r="Z570" s="6"/>
     </row>
-    <row r="571" spans="1:26" ht="30" customHeight="1">
+    <row r="571" spans="1:26" ht="14">
       <c r="A571" s="7"/>
       <c r="B571" s="16"/>
       <c r="C571" s="9"/>
@@ -16540,7 +16540,7 @@
       <c r="Y571" s="6"/>
       <c r="Z571" s="6"/>
     </row>
-    <row r="572" spans="1:26" ht="30" customHeight="1">
+    <row r="572" spans="1:26" ht="14">
       <c r="A572" s="7"/>
       <c r="B572" s="8"/>
       <c r="C572" s="9"/>
@@ -16568,7 +16568,7 @@
       <c r="Y572" s="6"/>
       <c r="Z572" s="6"/>
     </row>
-    <row r="573" spans="1:26" ht="30" customHeight="1">
+    <row r="573" spans="1:26" ht="14">
       <c r="A573" s="7"/>
       <c r="B573" s="8"/>
       <c r="C573" s="9"/>
@@ -16596,7 +16596,7 @@
       <c r="Y573" s="6"/>
       <c r="Z573" s="6"/>
     </row>
-    <row r="574" spans="1:26" ht="30" customHeight="1">
+    <row r="574" spans="1:26" ht="14">
       <c r="A574" s="7"/>
       <c r="B574" s="8"/>
       <c r="C574" s="9"/>
@@ -16624,7 +16624,7 @@
       <c r="Y574" s="6"/>
       <c r="Z574" s="6"/>
     </row>
-    <row r="575" spans="1:26" ht="30" customHeight="1">
+    <row r="575" spans="1:26" ht="14">
       <c r="A575" s="7"/>
       <c r="B575" s="8"/>
       <c r="C575" s="9"/>
@@ -16680,7 +16680,7 @@
       <c r="Y576" s="6"/>
       <c r="Z576" s="6"/>
     </row>
-    <row r="577" spans="1:26" ht="30" customHeight="1">
+    <row r="577" spans="1:26" ht="14">
       <c r="A577" s="7"/>
       <c r="B577" s="8"/>
       <c r="C577" s="9"/>
@@ -16764,7 +16764,7 @@
       <c r="Y579" s="6"/>
       <c r="Z579" s="6"/>
     </row>
-    <row r="580" spans="1:26" ht="30" customHeight="1">
+    <row r="580" spans="1:26" ht="14">
       <c r="A580" s="12"/>
       <c r="B580" s="13"/>
       <c r="C580" s="14"/>
@@ -16792,7 +16792,7 @@
       <c r="Y580" s="6"/>
       <c r="Z580" s="6"/>
     </row>
-    <row r="581" spans="1:26" ht="30" customHeight="1">
+    <row r="581" spans="1:26" ht="14">
       <c r="A581" s="12"/>
       <c r="B581" s="13"/>
       <c r="C581" s="14"/>
@@ -16848,7 +16848,7 @@
       <c r="Y582" s="6"/>
       <c r="Z582" s="6"/>
     </row>
-    <row r="583" spans="1:26" ht="30" customHeight="1">
+    <row r="583" spans="1:26" ht="14">
       <c r="A583" s="12"/>
       <c r="B583" s="13"/>
       <c r="C583" s="14"/>
@@ -16876,7 +16876,7 @@
       <c r="Y583" s="6"/>
       <c r="Z583" s="6"/>
     </row>
-    <row r="584" spans="1:26" ht="30" customHeight="1">
+    <row r="584" spans="1:26" ht="14">
       <c r="A584" s="12"/>
       <c r="B584" s="13"/>
       <c r="C584" s="14"/>
@@ -16932,7 +16932,7 @@
       <c r="Y585" s="6"/>
       <c r="Z585" s="6"/>
     </row>
-    <row r="586" spans="1:26" ht="30" customHeight="1">
+    <row r="586" spans="1:26" ht="14">
       <c r="A586" s="12"/>
       <c r="B586" s="13"/>
       <c r="C586" s="14"/>
@@ -16960,7 +16960,7 @@
       <c r="Y586" s="6"/>
       <c r="Z586" s="6"/>
     </row>
-    <row r="587" spans="1:26" ht="30" customHeight="1">
+    <row r="587" spans="1:26" ht="14">
       <c r="A587" s="12"/>
       <c r="B587" s="13"/>
       <c r="C587" s="14"/>
@@ -16988,7 +16988,7 @@
       <c r="Y587" s="6"/>
       <c r="Z587" s="6"/>
     </row>
-    <row r="588" spans="1:26" ht="30" customHeight="1">
+    <row r="588" spans="1:26" ht="14">
       <c r="A588" s="12"/>
       <c r="B588" s="13"/>
       <c r="C588" s="14"/>
@@ -17072,7 +17072,7 @@
       <c r="Y590" s="6"/>
       <c r="Z590" s="6"/>
     </row>
-    <row r="591" spans="1:26" ht="30" customHeight="1">
+    <row r="591" spans="1:26" ht="14">
       <c r="A591" s="12"/>
       <c r="B591" s="13"/>
       <c r="C591" s="14"/>
@@ -17128,7 +17128,7 @@
       <c r="Y592" s="6"/>
       <c r="Z592" s="6"/>
     </row>
-    <row r="593" spans="1:26" ht="60" customHeight="1">
+    <row r="593" spans="1:26" ht="14">
       <c r="A593" s="12"/>
       <c r="B593" s="13"/>
       <c r="C593" s="14"/>
@@ -17184,7 +17184,7 @@
       <c r="Y594" s="6"/>
       <c r="Z594" s="6"/>
     </row>
-    <row r="595" spans="1:26" ht="30" customHeight="1">
+    <row r="595" spans="1:26" ht="14">
       <c r="A595" s="7"/>
       <c r="B595" s="16"/>
       <c r="C595" s="9"/>
@@ -17380,7 +17380,7 @@
       <c r="Y601" s="6"/>
       <c r="Z601" s="6"/>
     </row>
-    <row r="602" spans="1:26" ht="30" customHeight="1">
+    <row r="602" spans="1:26" ht="14">
       <c r="A602" s="7"/>
       <c r="B602" s="16"/>
       <c r="C602" s="9"/>
@@ -17492,7 +17492,7 @@
       <c r="Y605" s="6"/>
       <c r="Z605" s="6"/>
     </row>
-    <row r="606" spans="1:26" ht="30" customHeight="1">
+    <row r="606" spans="1:26" ht="14">
       <c r="A606" s="7"/>
       <c r="B606" s="16"/>
       <c r="C606" s="9"/>
@@ -17548,7 +17548,7 @@
       <c r="Y607" s="6"/>
       <c r="Z607" s="6"/>
     </row>
-    <row r="608" spans="1:26" ht="30" customHeight="1">
+    <row r="608" spans="1:26" ht="14">
       <c r="A608" s="7"/>
       <c r="B608" s="16"/>
       <c r="C608" s="9"/>
@@ -17576,7 +17576,7 @@
       <c r="Y608" s="6"/>
       <c r="Z608" s="6"/>
     </row>
-    <row r="609" spans="1:26" ht="30" customHeight="1">
+    <row r="609" spans="1:26" ht="14">
       <c r="A609" s="7"/>
       <c r="B609" s="16"/>
       <c r="C609" s="9"/>
@@ -17604,7 +17604,7 @@
       <c r="Y609" s="6"/>
       <c r="Z609" s="6"/>
     </row>
-    <row r="610" spans="1:26" ht="30" customHeight="1">
+    <row r="610" spans="1:26" ht="14">
       <c r="A610" s="7"/>
       <c r="B610" s="16"/>
       <c r="C610" s="9"/>
@@ -17632,7 +17632,7 @@
       <c r="Y610" s="6"/>
       <c r="Z610" s="6"/>
     </row>
-    <row r="611" spans="1:26" ht="30" customHeight="1">
+    <row r="611" spans="1:26" ht="14">
       <c r="A611" s="7"/>
       <c r="B611" s="16"/>
       <c r="C611" s="9"/>
@@ -17660,7 +17660,7 @@
       <c r="Y611" s="6"/>
       <c r="Z611" s="6"/>
     </row>
-    <row r="612" spans="1:26" ht="30" customHeight="1">
+    <row r="612" spans="1:26" ht="14">
       <c r="A612" s="7"/>
       <c r="B612" s="16"/>
       <c r="C612" s="9"/>
@@ -17688,7 +17688,7 @@
       <c r="Y612" s="6"/>
       <c r="Z612" s="6"/>
     </row>
-    <row r="613" spans="1:26" ht="30" customHeight="1">
+    <row r="613" spans="1:26" ht="14">
       <c r="A613" s="7"/>
       <c r="B613" s="16"/>
       <c r="C613" s="9"/>
@@ -17716,7 +17716,7 @@
       <c r="Y613" s="6"/>
       <c r="Z613" s="6"/>
     </row>
-    <row r="614" spans="1:26" ht="30" customHeight="1">
+    <row r="614" spans="1:26" ht="14">
       <c r="A614" s="7"/>
       <c r="B614" s="16"/>
       <c r="C614" s="9"/>
@@ -17772,7 +17772,7 @@
       <c r="Y615" s="6"/>
       <c r="Z615" s="6"/>
     </row>
-    <row r="616" spans="1:26" ht="30" customHeight="1">
+    <row r="616" spans="1:26" ht="14">
       <c r="A616" s="7"/>
       <c r="B616" s="16"/>
       <c r="C616" s="9"/>
@@ -17828,7 +17828,7 @@
       <c r="Y617" s="6"/>
       <c r="Z617" s="6"/>
     </row>
-    <row r="618" spans="1:26" ht="30" customHeight="1">
+    <row r="618" spans="1:26" ht="14">
       <c r="A618" s="7"/>
       <c r="B618" s="16"/>
       <c r="C618" s="9"/>
@@ -17856,7 +17856,7 @@
       <c r="Y618" s="6"/>
       <c r="Z618" s="6"/>
     </row>
-    <row r="619" spans="1:26" ht="30" customHeight="1">
+    <row r="619" spans="1:26" ht="14">
       <c r="A619" s="7"/>
       <c r="B619" s="16"/>
       <c r="C619" s="9"/>
@@ -17884,7 +17884,7 @@
       <c r="Y619" s="6"/>
       <c r="Z619" s="6"/>
     </row>
-    <row r="620" spans="1:26" ht="30" customHeight="1">
+    <row r="620" spans="1:26" ht="14">
       <c r="A620" s="7"/>
       <c r="B620" s="16"/>
       <c r="C620" s="9"/>
@@ -17940,7 +17940,7 @@
       <c r="Y621" s="6"/>
       <c r="Z621" s="6"/>
     </row>
-    <row r="622" spans="1:26" ht="30" customHeight="1">
+    <row r="622" spans="1:26" ht="14">
       <c r="A622" s="7"/>
       <c r="B622" s="8"/>
       <c r="C622" s="9"/>
@@ -17996,7 +17996,7 @@
       <c r="Y623" s="6"/>
       <c r="Z623" s="6"/>
     </row>
-    <row r="624" spans="1:26" ht="30" customHeight="1">
+    <row r="624" spans="1:26" ht="14">
       <c r="A624" s="7"/>
       <c r="B624" s="8"/>
       <c r="C624" s="9"/>
@@ -18052,7 +18052,7 @@
       <c r="Y625" s="6"/>
       <c r="Z625" s="6"/>
     </row>
-    <row r="626" spans="1:26" ht="30" customHeight="1">
+    <row r="626" spans="1:26" ht="14">
       <c r="A626" s="12"/>
       <c r="B626" s="13"/>
       <c r="C626" s="14"/>
@@ -18136,7 +18136,7 @@
       <c r="Y628" s="6"/>
       <c r="Z628" s="6"/>
     </row>
-    <row r="629" spans="1:26" ht="30" customHeight="1">
+    <row r="629" spans="1:26" ht="14">
       <c r="A629" s="12"/>
       <c r="B629" s="13"/>
       <c r="C629" s="14"/>
@@ -18164,7 +18164,7 @@
       <c r="Y629" s="6"/>
       <c r="Z629" s="6"/>
     </row>
-    <row r="630" spans="1:26" ht="30" customHeight="1">
+    <row r="630" spans="1:26" ht="14">
       <c r="A630" s="12"/>
       <c r="B630" s="13"/>
       <c r="C630" s="14"/>
@@ -18192,7 +18192,7 @@
       <c r="Y630" s="6"/>
       <c r="Z630" s="6"/>
     </row>
-    <row r="631" spans="1:26" ht="30" customHeight="1">
+    <row r="631" spans="1:26" ht="14">
       <c r="A631" s="12"/>
       <c r="B631" s="13"/>
       <c r="C631" s="14"/>
@@ -18220,7 +18220,7 @@
       <c r="Y631" s="6"/>
       <c r="Z631" s="6"/>
     </row>
-    <row r="632" spans="1:26" ht="30" customHeight="1">
+    <row r="632" spans="1:26" ht="14">
       <c r="A632" s="12"/>
       <c r="B632" s="13"/>
       <c r="C632" s="14"/>
@@ -18248,7 +18248,7 @@
       <c r="Y632" s="6"/>
       <c r="Z632" s="6"/>
     </row>
-    <row r="633" spans="1:26" ht="30" customHeight="1">
+    <row r="633" spans="1:26" ht="14">
       <c r="A633" s="17"/>
       <c r="B633" s="18"/>
       <c r="C633" s="14"/>
@@ -18332,7 +18332,7 @@
       <c r="Y635" s="6"/>
       <c r="Z635" s="6"/>
     </row>
-    <row r="636" spans="1:26" ht="30" customHeight="1">
+    <row r="636" spans="1:26" ht="14">
       <c r="A636" s="7"/>
       <c r="B636" s="16"/>
       <c r="C636" s="9"/>
@@ -18388,7 +18388,7 @@
       <c r="Y637" s="6"/>
       <c r="Z637" s="6"/>
     </row>
-    <row r="638" spans="1:26" ht="30" customHeight="1">
+    <row r="638" spans="1:26" ht="14">
       <c r="A638" s="7"/>
       <c r="B638" s="16"/>
       <c r="C638" s="9"/>
@@ -18416,7 +18416,7 @@
       <c r="Y638" s="6"/>
       <c r="Z638" s="6"/>
     </row>
-    <row r="639" spans="1:26" ht="30" customHeight="1">
+    <row r="639" spans="1:26" ht="14">
       <c r="A639" s="7"/>
       <c r="B639" s="16"/>
       <c r="C639" s="9"/>
@@ -18444,7 +18444,7 @@
       <c r="Y639" s="6"/>
       <c r="Z639" s="6"/>
     </row>
-    <row r="640" spans="1:26" ht="30" customHeight="1">
+    <row r="640" spans="1:26" ht="14">
       <c r="A640" s="7"/>
       <c r="B640" s="16"/>
       <c r="C640" s="9"/>
@@ -18500,7 +18500,7 @@
       <c r="Y641" s="6"/>
       <c r="Z641" s="6"/>
     </row>
-    <row r="642" spans="1:26" ht="30" customHeight="1">
+    <row r="642" spans="1:26" ht="14">
       <c r="A642" s="7"/>
       <c r="B642" s="16"/>
       <c r="C642" s="9"/>
@@ -18584,7 +18584,7 @@
       <c r="Y644" s="6"/>
       <c r="Z644" s="6"/>
     </row>
-    <row r="645" spans="1:26" ht="30" customHeight="1">
+    <row r="645" spans="1:26" ht="14">
       <c r="A645" s="7"/>
       <c r="B645" s="16"/>
       <c r="C645" s="9"/>
@@ -18612,7 +18612,7 @@
       <c r="Y645" s="6"/>
       <c r="Z645" s="6"/>
     </row>
-    <row r="646" spans="1:26" ht="30" customHeight="1">
+    <row r="646" spans="1:26" ht="14">
       <c r="A646" s="7"/>
       <c r="B646" s="16"/>
       <c r="C646" s="9"/>
@@ -18668,7 +18668,7 @@
       <c r="Y647" s="6"/>
       <c r="Z647" s="6"/>
     </row>
-    <row r="648" spans="1:26" ht="30" customHeight="1">
+    <row r="648" spans="1:26" ht="14">
       <c r="A648" s="7"/>
       <c r="B648" s="16"/>
       <c r="C648" s="9"/>
@@ -18696,7 +18696,7 @@
       <c r="Y648" s="6"/>
       <c r="Z648" s="6"/>
     </row>
-    <row r="649" spans="1:26" ht="30" customHeight="1">
+    <row r="649" spans="1:26" ht="14">
       <c r="A649" s="7"/>
       <c r="B649" s="16"/>
       <c r="C649" s="9"/>
@@ -18724,7 +18724,7 @@
       <c r="Y649" s="6"/>
       <c r="Z649" s="6"/>
     </row>
-    <row r="650" spans="1:26" ht="30" customHeight="1">
+    <row r="650" spans="1:26" ht="14">
       <c r="A650" s="7"/>
       <c r="B650" s="16"/>
       <c r="C650" s="9"/>
@@ -18752,7 +18752,7 @@
       <c r="Y650" s="6"/>
       <c r="Z650" s="6"/>
     </row>
-    <row r="651" spans="1:26" ht="30" customHeight="1">
+    <row r="651" spans="1:26" ht="14">
       <c r="A651" s="7"/>
       <c r="B651" s="16"/>
       <c r="C651" s="9"/>
@@ -18780,7 +18780,7 @@
       <c r="Y651" s="6"/>
       <c r="Z651" s="6"/>
     </row>
-    <row r="652" spans="1:26" ht="30" customHeight="1">
+    <row r="652" spans="1:26" ht="14">
       <c r="A652" s="7"/>
       <c r="B652" s="16"/>
       <c r="C652" s="9"/>
@@ -18808,7 +18808,7 @@
       <c r="Y652" s="6"/>
       <c r="Z652" s="6"/>
     </row>
-    <row r="653" spans="1:26" ht="30" customHeight="1">
+    <row r="653" spans="1:26" ht="14">
       <c r="A653" s="7"/>
       <c r="B653" s="16"/>
       <c r="C653" s="9"/>
@@ -18864,7 +18864,7 @@
       <c r="Y654" s="6"/>
       <c r="Z654" s="6"/>
     </row>
-    <row r="655" spans="1:26" ht="30" customHeight="1">
+    <row r="655" spans="1:26" ht="14">
       <c r="A655" s="7"/>
       <c r="B655" s="16"/>
       <c r="C655" s="9"/>
@@ -18892,7 +18892,7 @@
       <c r="Y655" s="6"/>
       <c r="Z655" s="6"/>
     </row>
-    <row r="656" spans="1:26" ht="30" customHeight="1">
+    <row r="656" spans="1:26" ht="14">
       <c r="A656" s="7"/>
       <c r="B656" s="16"/>
       <c r="C656" s="9"/>
@@ -18948,7 +18948,7 @@
       <c r="Y657" s="6"/>
       <c r="Z657" s="6"/>
     </row>
-    <row r="658" spans="1:26" ht="30" customHeight="1">
+    <row r="658" spans="1:26" ht="14">
       <c r="A658" s="7"/>
       <c r="B658" s="8"/>
       <c r="C658" s="9"/>
@@ -18976,7 +18976,7 @@
       <c r="Y658" s="6"/>
       <c r="Z658" s="6"/>
     </row>
-    <row r="659" spans="1:26" ht="30" customHeight="1">
+    <row r="659" spans="1:26" ht="14">
       <c r="A659" s="7"/>
       <c r="B659" s="8"/>
       <c r="C659" s="9"/>
@@ -19060,7 +19060,7 @@
       <c r="Y661" s="6"/>
       <c r="Z661" s="6"/>
     </row>
-    <row r="662" spans="1:26" ht="30" customHeight="1">
+    <row r="662" spans="1:26" ht="14">
       <c r="A662" s="7"/>
       <c r="B662" s="8"/>
       <c r="C662" s="9"/>
@@ -19144,7 +19144,7 @@
       <c r="Y664" s="6"/>
       <c r="Z664" s="6"/>
     </row>
-    <row r="665" spans="1:26" ht="30" customHeight="1">
+    <row r="665" spans="1:26" ht="14">
       <c r="A665" s="12"/>
       <c r="B665" s="13"/>
       <c r="C665" s="14"/>
@@ -19172,7 +19172,7 @@
       <c r="Y665" s="6"/>
       <c r="Z665" s="6"/>
     </row>
-    <row r="666" spans="1:26" ht="30" customHeight="1">
+    <row r="666" spans="1:26" ht="14">
       <c r="A666" s="12"/>
       <c r="B666" s="13"/>
       <c r="C666" s="14"/>
@@ -19228,7 +19228,7 @@
       <c r="Y667" s="6"/>
       <c r="Z667" s="6"/>
     </row>
-    <row r="668" spans="1:26" ht="30" customHeight="1">
+    <row r="668" spans="1:26" ht="14">
       <c r="A668" s="12"/>
       <c r="B668" s="13"/>
       <c r="C668" s="14"/>
@@ -19284,7 +19284,7 @@
       <c r="Y669" s="6"/>
       <c r="Z669" s="6"/>
     </row>
-    <row r="670" spans="1:26" ht="30" customHeight="1">
+    <row r="670" spans="1:26" ht="14">
       <c r="A670" s="12"/>
       <c r="B670" s="13"/>
       <c r="C670" s="14"/>
@@ -19312,7 +19312,7 @@
       <c r="Y670" s="6"/>
       <c r="Z670" s="6"/>
     </row>
-    <row r="671" spans="1:26" ht="30" customHeight="1">
+    <row r="671" spans="1:26" ht="14">
       <c r="A671" s="12"/>
       <c r="B671" s="13"/>
       <c r="C671" s="14"/>
@@ -19396,7 +19396,7 @@
       <c r="Y673" s="6"/>
       <c r="Z673" s="6"/>
     </row>
-    <row r="674" spans="1:26" ht="30" customHeight="1">
+    <row r="674" spans="1:26" ht="14">
       <c r="A674" s="7"/>
       <c r="B674" s="16"/>
       <c r="C674" s="9"/>
@@ -19424,7 +19424,7 @@
       <c r="Y674" s="6"/>
       <c r="Z674" s="6"/>
     </row>
-    <row r="675" spans="1:26" ht="30" customHeight="1">
+    <row r="675" spans="1:26" ht="14">
       <c r="A675" s="7"/>
       <c r="B675" s="16"/>
       <c r="C675" s="9"/>
@@ -19480,7 +19480,7 @@
       <c r="Y676" s="6"/>
       <c r="Z676" s="6"/>
     </row>
-    <row r="677" spans="1:26" ht="30" customHeight="1">
+    <row r="677" spans="1:26" ht="14">
       <c r="A677" s="7"/>
       <c r="B677" s="16"/>
       <c r="C677" s="9"/>
@@ -19508,7 +19508,7 @@
       <c r="Y677" s="6"/>
       <c r="Z677" s="6"/>
     </row>
-    <row r="678" spans="1:26" ht="30" customHeight="1">
+    <row r="678" spans="1:26" ht="14">
       <c r="A678" s="7"/>
       <c r="B678" s="16"/>
       <c r="C678" s="9"/>
@@ -19536,7 +19536,7 @@
       <c r="Y678" s="6"/>
       <c r="Z678" s="6"/>
     </row>
-    <row r="679" spans="1:26" ht="30" customHeight="1">
+    <row r="679" spans="1:26" ht="14">
       <c r="A679" s="7"/>
       <c r="B679" s="16"/>
       <c r="C679" s="9"/>
@@ -19592,7 +19592,7 @@
       <c r="Y680" s="6"/>
       <c r="Z680" s="6"/>
     </row>
-    <row r="681" spans="1:26" ht="30" customHeight="1">
+    <row r="681" spans="1:26" ht="14">
       <c r="A681" s="7"/>
       <c r="B681" s="16"/>
       <c r="C681" s="9"/>
@@ -19648,7 +19648,7 @@
       <c r="Y682" s="6"/>
       <c r="Z682" s="6"/>
     </row>
-    <row r="683" spans="1:26" ht="30" customHeight="1">
+    <row r="683" spans="1:26" ht="14">
       <c r="A683" s="7"/>
       <c r="B683" s="16"/>
       <c r="C683" s="9"/>
@@ -19704,7 +19704,7 @@
       <c r="Y684" s="6"/>
       <c r="Z684" s="6"/>
     </row>
-    <row r="685" spans="1:26" ht="30" customHeight="1">
+    <row r="685" spans="1:26" ht="14">
       <c r="A685" s="7"/>
       <c r="B685" s="16"/>
       <c r="C685" s="9"/>
@@ -19732,7 +19732,7 @@
       <c r="Y685" s="6"/>
       <c r="Z685" s="6"/>
     </row>
-    <row r="686" spans="1:26" ht="30" customHeight="1">
+    <row r="686" spans="1:26" ht="14">
       <c r="A686" s="7"/>
       <c r="B686" s="16"/>
       <c r="C686" s="9"/>
@@ -19760,7 +19760,7 @@
       <c r="Y686" s="6"/>
       <c r="Z686" s="6"/>
     </row>
-    <row r="687" spans="1:26" ht="30" customHeight="1">
+    <row r="687" spans="1:26" ht="14">
       <c r="A687" s="7"/>
       <c r="B687" s="16"/>
       <c r="C687" s="9"/>
@@ -19788,7 +19788,7 @@
       <c r="Y687" s="6"/>
       <c r="Z687" s="6"/>
     </row>
-    <row r="688" spans="1:26" ht="30" customHeight="1">
+    <row r="688" spans="1:26" ht="14">
       <c r="A688" s="7"/>
       <c r="B688" s="16"/>
       <c r="C688" s="9"/>
@@ -19872,7 +19872,7 @@
       <c r="Y690" s="6"/>
       <c r="Z690" s="6"/>
     </row>
-    <row r="691" spans="1:26" ht="30" customHeight="1">
+    <row r="691" spans="1:26" ht="14">
       <c r="A691" s="12"/>
       <c r="B691" s="13"/>
       <c r="C691" s="14"/>
@@ -19928,7 +19928,7 @@
       <c r="Y692" s="6"/>
       <c r="Z692" s="6"/>
     </row>
-    <row r="693" spans="1:26" ht="30" customHeight="1">
+    <row r="693" spans="1:26" ht="14">
       <c r="A693" s="7"/>
       <c r="B693" s="16"/>
       <c r="C693" s="9"/>
@@ -20012,7 +20012,7 @@
       <c r="Y695" s="6"/>
       <c r="Z695" s="6"/>
     </row>
-    <row r="696" spans="1:26" ht="30" customHeight="1">
+    <row r="696" spans="1:26" ht="14">
       <c r="A696" s="7"/>
       <c r="B696" s="16"/>
       <c r="C696" s="9"/>
@@ -20068,7 +20068,7 @@
       <c r="Y697" s="6"/>
       <c r="Z697" s="6"/>
     </row>
-    <row r="698" spans="1:26" ht="30" customHeight="1">
+    <row r="698" spans="1:26" ht="14">
       <c r="A698" s="7"/>
       <c r="B698" s="16"/>
       <c r="C698" s="9"/>
@@ -20096,7 +20096,7 @@
       <c r="Y698" s="6"/>
       <c r="Z698" s="6"/>
     </row>
-    <row r="699" spans="1:26" ht="30" customHeight="1">
+    <row r="699" spans="1:26" ht="14">
       <c r="A699" s="7"/>
       <c r="B699" s="16"/>
       <c r="C699" s="9"/>
@@ -20124,7 +20124,7 @@
       <c r="Y699" s="6"/>
       <c r="Z699" s="6"/>
     </row>
-    <row r="700" spans="1:26" ht="30" customHeight="1">
+    <row r="700" spans="1:26" ht="14">
       <c r="A700" s="7"/>
       <c r="B700" s="16"/>
       <c r="C700" s="9"/>
@@ -20152,7 +20152,7 @@
       <c r="Y700" s="6"/>
       <c r="Z700" s="6"/>
     </row>
-    <row r="701" spans="1:26" ht="30" customHeight="1">
+    <row r="701" spans="1:26" ht="14">
       <c r="A701" s="7"/>
       <c r="B701" s="16"/>
       <c r="C701" s="9"/>
@@ -20180,7 +20180,7 @@
       <c r="Y701" s="6"/>
       <c r="Z701" s="6"/>
     </row>
-    <row r="702" spans="1:26" ht="30" customHeight="1">
+    <row r="702" spans="1:26" ht="14">
       <c r="A702" s="7"/>
       <c r="B702" s="16"/>
       <c r="C702" s="9"/>
@@ -20236,7 +20236,7 @@
       <c r="Y703" s="6"/>
       <c r="Z703" s="6"/>
     </row>
-    <row r="704" spans="1:26" ht="30" customHeight="1">
+    <row r="704" spans="1:26" ht="14">
       <c r="A704" s="7"/>
       <c r="B704" s="16"/>
       <c r="C704" s="9"/>
@@ -20264,7 +20264,7 @@
       <c r="Y704" s="6"/>
       <c r="Z704" s="6"/>
     </row>
-    <row r="705" spans="1:26" ht="30" customHeight="1">
+    <row r="705" spans="1:26" ht="14">
       <c r="A705" s="7"/>
       <c r="B705" s="8"/>
       <c r="C705" s="9"/>
@@ -20292,7 +20292,7 @@
       <c r="Y705" s="6"/>
       <c r="Z705" s="6"/>
     </row>
-    <row r="706" spans="1:26" ht="30" customHeight="1">
+    <row r="706" spans="1:26" ht="14">
       <c r="A706" s="12"/>
       <c r="B706" s="13"/>
       <c r="C706" s="14"/>
@@ -20376,7 +20376,7 @@
       <c r="Y708" s="6"/>
       <c r="Z708" s="6"/>
     </row>
-    <row r="709" spans="1:26" ht="30" customHeight="1">
+    <row r="709" spans="1:26" ht="14">
       <c r="A709" s="7"/>
       <c r="B709" s="16"/>
       <c r="C709" s="9"/>
@@ -20432,7 +20432,7 @@
       <c r="Y710" s="6"/>
       <c r="Z710" s="6"/>
     </row>
-    <row r="711" spans="1:26" ht="30" customHeight="1">
+    <row r="711" spans="1:26" ht="14">
       <c r="A711" s="7"/>
       <c r="B711" s="16"/>
       <c r="C711" s="9"/>
@@ -20460,7 +20460,7 @@
       <c r="Y711" s="6"/>
       <c r="Z711" s="6"/>
     </row>
-    <row r="712" spans="1:26" ht="30" customHeight="1">
+    <row r="712" spans="1:26" ht="14">
       <c r="A712" s="7"/>
       <c r="B712" s="16"/>
       <c r="C712" s="9"/>
@@ -20488,7 +20488,7 @@
       <c r="Y712" s="6"/>
       <c r="Z712" s="6"/>
     </row>
-    <row r="713" spans="1:26" ht="30" customHeight="1">
+    <row r="713" spans="1:26" ht="14">
       <c r="A713" s="7"/>
       <c r="B713" s="16"/>
       <c r="C713" s="9"/>
@@ -20516,7 +20516,7 @@
       <c r="Y713" s="6"/>
       <c r="Z713" s="6"/>
     </row>
-    <row r="714" spans="1:26" ht="30" customHeight="1">
+    <row r="714" spans="1:26" ht="14">
       <c r="A714" s="7"/>
       <c r="B714" s="16"/>
       <c r="C714" s="9"/>
@@ -20544,7 +20544,7 @@
       <c r="Y714" s="6"/>
       <c r="Z714" s="6"/>
     </row>
-    <row r="715" spans="1:26" ht="30" customHeight="1">
+    <row r="715" spans="1:26" ht="14">
       <c r="A715" s="7"/>
       <c r="B715" s="16"/>
       <c r="C715" s="9"/>
@@ -20600,7 +20600,7 @@
       <c r="Y716" s="6"/>
       <c r="Z716" s="6"/>
     </row>
-    <row r="717" spans="1:26" ht="30" customHeight="1">
+    <row r="717" spans="1:26" ht="14">
       <c r="A717" s="7"/>
       <c r="B717" s="16"/>
       <c r="C717" s="9"/>
@@ -20628,7 +20628,7 @@
       <c r="Y717" s="6"/>
       <c r="Z717" s="6"/>
     </row>
-    <row r="718" spans="1:26" ht="30" customHeight="1">
+    <row r="718" spans="1:26" ht="14">
       <c r="A718" s="7"/>
       <c r="B718" s="16"/>
       <c r="C718" s="9"/>
@@ -20656,7 +20656,7 @@
       <c r="Y718" s="6"/>
       <c r="Z718" s="6"/>
     </row>
-    <row r="719" spans="1:26" ht="30" customHeight="1">
+    <row r="719" spans="1:26" ht="14">
       <c r="A719" s="7"/>
       <c r="B719" s="16"/>
       <c r="C719" s="9"/>
@@ -20684,7 +20684,7 @@
       <c r="Y719" s="6"/>
       <c r="Z719" s="6"/>
     </row>
-    <row r="720" spans="1:26" ht="30" customHeight="1">
+    <row r="720" spans="1:26" ht="14">
       <c r="A720" s="7"/>
       <c r="B720" s="16"/>
       <c r="C720" s="9"/>
@@ -20740,7 +20740,7 @@
       <c r="Y721" s="6"/>
       <c r="Z721" s="6"/>
     </row>
-    <row r="722" spans="1:26" ht="30" customHeight="1">
+    <row r="722" spans="1:26" ht="14">
       <c r="A722" s="7"/>
       <c r="B722" s="16"/>
       <c r="C722" s="9"/>
@@ -20768,7 +20768,7 @@
       <c r="Y722" s="6"/>
       <c r="Z722" s="6"/>
     </row>
-    <row r="723" spans="1:26" ht="30" customHeight="1">
+    <row r="723" spans="1:26" ht="14">
       <c r="A723" s="7"/>
       <c r="B723" s="16"/>
       <c r="C723" s="9"/>
@@ -20824,7 +20824,7 @@
       <c r="Y724" s="6"/>
       <c r="Z724" s="6"/>
     </row>
-    <row r="725" spans="1:26" ht="30" customHeight="1">
+    <row r="725" spans="1:26" ht="14">
       <c r="A725" s="7"/>
       <c r="B725" s="8"/>
       <c r="C725" s="9"/>
@@ -20880,7 +20880,7 @@
       <c r="Y726" s="6"/>
       <c r="Z726" s="6"/>
     </row>
-    <row r="727" spans="1:26" ht="30" customHeight="1">
+    <row r="727" spans="1:26" ht="14">
       <c r="A727" s="7"/>
       <c r="B727" s="8"/>
       <c r="C727" s="9"/>
@@ -20908,7 +20908,7 @@
       <c r="Y727" s="6"/>
       <c r="Z727" s="6"/>
     </row>
-    <row r="728" spans="1:26" ht="30" customHeight="1">
+    <row r="728" spans="1:26" ht="14">
       <c r="A728" s="12"/>
       <c r="B728" s="13"/>
       <c r="C728" s="14"/>
@@ -20936,7 +20936,7 @@
       <c r="Y728" s="6"/>
       <c r="Z728" s="6"/>
     </row>
-    <row r="729" spans="1:26" ht="30" customHeight="1">
+    <row r="729" spans="1:26" ht="14">
       <c r="A729" s="12"/>
       <c r="B729" s="13"/>
       <c r="C729" s="14"/>
@@ -20964,7 +20964,7 @@
       <c r="Y729" s="6"/>
       <c r="Z729" s="6"/>
     </row>
-    <row r="730" spans="1:26" ht="30" customHeight="1">
+    <row r="730" spans="1:26" ht="14">
       <c r="A730" s="12"/>
       <c r="B730" s="13"/>
       <c r="C730" s="14"/>
@@ -20992,7 +20992,7 @@
       <c r="Y730" s="6"/>
       <c r="Z730" s="6"/>
     </row>
-    <row r="731" spans="1:26" ht="30" customHeight="1">
+    <row r="731" spans="1:26" ht="14">
       <c r="A731" s="12"/>
       <c r="B731" s="13"/>
       <c r="C731" s="14"/>
@@ -21020,7 +21020,7 @@
       <c r="Y731" s="6"/>
       <c r="Z731" s="6"/>
     </row>
-    <row r="732" spans="1:26" ht="30" customHeight="1">
+    <row r="732" spans="1:26" ht="14">
       <c r="A732" s="12"/>
       <c r="B732" s="13"/>
       <c r="C732" s="14"/>
@@ -21048,7 +21048,7 @@
       <c r="Y732" s="6"/>
       <c r="Z732" s="6"/>
     </row>
-    <row r="733" spans="1:26" ht="30" customHeight="1">
+    <row r="733" spans="1:26" ht="14">
       <c r="A733" s="12"/>
       <c r="B733" s="13"/>
       <c r="C733" s="14"/>
@@ -21076,7 +21076,7 @@
       <c r="Y733" s="6"/>
       <c r="Z733" s="6"/>
     </row>
-    <row r="734" spans="1:26" ht="30" customHeight="1">
+    <row r="734" spans="1:26" ht="14">
       <c r="A734" s="12"/>
       <c r="B734" s="13"/>
       <c r="C734" s="14"/>
@@ -21160,7 +21160,7 @@
       <c r="Y736" s="6"/>
       <c r="Z736" s="6"/>
     </row>
-    <row r="737" spans="1:26" ht="30" customHeight="1">
+    <row r="737" spans="1:26" ht="14">
       <c r="A737" s="7"/>
       <c r="B737" s="8"/>
       <c r="C737" s="9"/>
@@ -21244,7 +21244,7 @@
       <c r="Y739" s="6"/>
       <c r="Z739" s="6"/>
     </row>
-    <row r="740" spans="1:26" ht="30" customHeight="1">
+    <row r="740" spans="1:26" ht="14">
       <c r="A740" s="7"/>
       <c r="B740" s="8"/>
       <c r="C740" s="9"/>
@@ -21300,7 +21300,7 @@
       <c r="Y741" s="6"/>
       <c r="Z741" s="6"/>
     </row>
-    <row r="742" spans="1:26" ht="30" customHeight="1">
+    <row r="742" spans="1:26" ht="14">
       <c r="A742" s="7"/>
       <c r="B742" s="8"/>
       <c r="C742" s="9"/>
@@ -21328,7 +21328,7 @@
       <c r="Y742" s="6"/>
       <c r="Z742" s="6"/>
     </row>
-    <row r="743" spans="1:26" ht="30" customHeight="1">
+    <row r="743" spans="1:26" ht="14">
       <c r="A743" s="7"/>
       <c r="B743" s="8"/>
       <c r="C743" s="9"/>
@@ -21356,7 +21356,7 @@
       <c r="Y743" s="6"/>
       <c r="Z743" s="6"/>
     </row>
-    <row r="744" spans="1:26" ht="30" customHeight="1">
+    <row r="744" spans="1:26" ht="14">
       <c r="A744" s="7"/>
       <c r="B744" s="8"/>
       <c r="C744" s="9"/>
@@ -21384,7 +21384,7 @@
       <c r="Y744" s="6"/>
       <c r="Z744" s="6"/>
     </row>
-    <row r="745" spans="1:26" ht="30" customHeight="1">
+    <row r="745" spans="1:26" ht="14">
       <c r="A745" s="7"/>
       <c r="B745" s="8"/>
       <c r="C745" s="9"/>
@@ -21440,7 +21440,7 @@
       <c r="Y746" s="6"/>
       <c r="Z746" s="6"/>
     </row>
-    <row r="747" spans="1:26" ht="30" customHeight="1">
+    <row r="747" spans="1:26" ht="14">
       <c r="A747" s="7"/>
       <c r="B747" s="8"/>
       <c r="C747" s="9"/>
@@ -21468,7 +21468,7 @@
       <c r="Y747" s="6"/>
       <c r="Z747" s="6"/>
     </row>
-    <row r="748" spans="1:26" ht="30" customHeight="1">
+    <row r="748" spans="1:26" ht="14">
       <c r="A748" s="7"/>
       <c r="B748" s="8"/>
       <c r="C748" s="9"/>
@@ -21496,7 +21496,7 @@
       <c r="Y748" s="6"/>
       <c r="Z748" s="6"/>
     </row>
-    <row r="749" spans="1:26" ht="30" customHeight="1">
+    <row r="749" spans="1:26" ht="14">
       <c r="A749" s="7"/>
       <c r="B749" s="8"/>
       <c r="C749" s="9"/>
@@ -21524,7 +21524,7 @@
       <c r="Y749" s="6"/>
       <c r="Z749" s="6"/>
     </row>
-    <row r="750" spans="1:26" ht="30" customHeight="1">
+    <row r="750" spans="1:26" ht="14">
       <c r="A750" s="7"/>
       <c r="B750" s="8"/>
       <c r="C750" s="9"/>
@@ -21552,7 +21552,7 @@
       <c r="Y750" s="6"/>
       <c r="Z750" s="6"/>
     </row>
-    <row r="751" spans="1:26" ht="30" customHeight="1">
+    <row r="751" spans="1:26" ht="14">
       <c r="A751" s="7"/>
       <c r="B751" s="8"/>
       <c r="C751" s="9"/>
@@ -21580,7 +21580,7 @@
       <c r="Y751" s="6"/>
       <c r="Z751" s="6"/>
     </row>
-    <row r="752" spans="1:26" ht="30" customHeight="1">
+    <row r="752" spans="1:26" ht="14">
       <c r="A752" s="7"/>
       <c r="B752" s="8"/>
       <c r="C752" s="9"/>
@@ -21608,7 +21608,7 @@
       <c r="Y752" s="6"/>
       <c r="Z752" s="6"/>
     </row>
-    <row r="753" spans="1:26" ht="30" customHeight="1">
+    <row r="753" spans="1:26" ht="14">
       <c r="A753" s="7"/>
       <c r="B753" s="8"/>
       <c r="C753" s="9"/>
@@ -21692,7 +21692,7 @@
       <c r="Y755" s="6"/>
       <c r="Z755" s="6"/>
     </row>
-    <row r="756" spans="1:26" ht="30" customHeight="1">
+    <row r="756" spans="1:26" ht="14">
       <c r="A756" s="7"/>
       <c r="B756" s="8"/>
       <c r="C756" s="9"/>
@@ -21748,7 +21748,7 @@
       <c r="Y757" s="6"/>
       <c r="Z757" s="6"/>
     </row>
-    <row r="758" spans="1:26" ht="30" customHeight="1">
+    <row r="758" spans="1:26" ht="14">
       <c r="A758" s="7"/>
       <c r="B758" s="8"/>
       <c r="C758" s="9"/>
@@ -21860,7 +21860,7 @@
       <c r="Y761" s="6"/>
       <c r="Z761" s="6"/>
     </row>
-    <row r="762" spans="1:26" ht="30" customHeight="1">
+    <row r="762" spans="1:26" ht="14">
       <c r="A762" s="12"/>
       <c r="B762" s="13"/>
       <c r="C762" s="14"/>
@@ -21888,7 +21888,7 @@
       <c r="Y762" s="6"/>
       <c r="Z762" s="6"/>
     </row>
-    <row r="763" spans="1:26" ht="30" customHeight="1">
+    <row r="763" spans="1:26" ht="14">
       <c r="A763" s="12"/>
       <c r="B763" s="13"/>
       <c r="C763" s="14"/>
@@ -21916,7 +21916,7 @@
       <c r="Y763" s="6"/>
       <c r="Z763" s="6"/>
     </row>
-    <row r="764" spans="1:26" ht="30" customHeight="1">
+    <row r="764" spans="1:26" ht="14">
       <c r="A764" s="12"/>
       <c r="B764" s="13"/>
       <c r="C764" s="14"/>
@@ -21944,7 +21944,7 @@
       <c r="Y764" s="6"/>
       <c r="Z764" s="6"/>
     </row>
-    <row r="765" spans="1:26" ht="30" customHeight="1">
+    <row r="765" spans="1:26" ht="14">
       <c r="A765" s="7"/>
       <c r="B765" s="8"/>
       <c r="C765" s="9"/>
@@ -22000,7 +22000,7 @@
       <c r="Y766" s="6"/>
       <c r="Z766" s="6"/>
     </row>
-    <row r="767" spans="1:26" ht="30" customHeight="1">
+    <row r="767" spans="1:26" ht="14">
       <c r="A767" s="7"/>
       <c r="B767" s="8"/>
       <c r="C767" s="9"/>
@@ -22084,7 +22084,7 @@
       <c r="Y769" s="6"/>
       <c r="Z769" s="6"/>
     </row>
-    <row r="770" spans="1:26" ht="30" customHeight="1">
+    <row r="770" spans="1:26" ht="14">
       <c r="A770" s="7"/>
       <c r="B770" s="8"/>
       <c r="C770" s="9"/>
@@ -22112,7 +22112,7 @@
       <c r="Y770" s="6"/>
       <c r="Z770" s="6"/>
     </row>
-    <row r="771" spans="1:26" ht="30" customHeight="1">
+    <row r="771" spans="1:26" ht="14">
       <c r="A771" s="7"/>
       <c r="B771" s="8"/>
       <c r="C771" s="9"/>
@@ -22140,7 +22140,7 @@
       <c r="Y771" s="6"/>
       <c r="Z771" s="6"/>
     </row>
-    <row r="772" spans="1:26" ht="30" customHeight="1">
+    <row r="772" spans="1:26" ht="14">
       <c r="A772" s="7"/>
       <c r="B772" s="8"/>
       <c r="C772" s="9"/>
@@ -22168,7 +22168,7 @@
       <c r="Y772" s="6"/>
       <c r="Z772" s="6"/>
     </row>
-    <row r="773" spans="1:26" ht="30" customHeight="1">
+    <row r="773" spans="1:26" ht="14">
       <c r="A773" s="7"/>
       <c r="B773" s="8"/>
       <c r="C773" s="9"/>
@@ -22196,7 +22196,7 @@
       <c r="Y773" s="6"/>
       <c r="Z773" s="6"/>
     </row>
-    <row r="774" spans="1:26" ht="30" customHeight="1">
+    <row r="774" spans="1:26" ht="14">
       <c r="A774" s="7"/>
       <c r="B774" s="8"/>
       <c r="C774" s="9"/>
@@ -22224,7 +22224,7 @@
       <c r="Y774" s="6"/>
       <c r="Z774" s="6"/>
     </row>
-    <row r="775" spans="1:26" ht="30" customHeight="1">
+    <row r="775" spans="1:26" ht="14">
       <c r="A775" s="7"/>
       <c r="B775" s="8"/>
       <c r="C775" s="9"/>
@@ -22252,7 +22252,7 @@
       <c r="Y775" s="6"/>
       <c r="Z775" s="6"/>
     </row>
-    <row r="776" spans="1:26" ht="30" customHeight="1">
+    <row r="776" spans="1:26" ht="14">
       <c r="A776" s="7"/>
       <c r="B776" s="8"/>
       <c r="C776" s="9"/>
@@ -22280,7 +22280,7 @@
       <c r="Y776" s="6"/>
       <c r="Z776" s="6"/>
     </row>
-    <row r="777" spans="1:26" ht="30" customHeight="1">
+    <row r="777" spans="1:26" ht="14">
       <c r="A777" s="7"/>
       <c r="B777" s="8"/>
       <c r="C777" s="9"/>
@@ -22308,7 +22308,7 @@
       <c r="Y777" s="6"/>
       <c r="Z777" s="6"/>
     </row>
-    <row r="778" spans="1:26" ht="30" customHeight="1">
+    <row r="778" spans="1:26" ht="14">
       <c r="A778" s="7"/>
       <c r="B778" s="8"/>
       <c r="C778" s="9"/>
@@ -22392,7 +22392,7 @@
       <c r="Y780" s="6"/>
       <c r="Z780" s="6"/>
     </row>
-    <row r="781" spans="1:26" ht="30" customHeight="1">
+    <row r="781" spans="1:26" ht="14">
       <c r="A781" s="7"/>
       <c r="B781" s="8"/>
       <c r="C781" s="9"/>
@@ -22448,7 +22448,7 @@
       <c r="Y782" s="6"/>
       <c r="Z782" s="6"/>
     </row>
-    <row r="783" spans="1:26" ht="60" customHeight="1">
+    <row r="783" spans="1:26" ht="14">
       <c r="A783" s="12"/>
       <c r="B783" s="13"/>
       <c r="C783" s="14"/>
@@ -22504,7 +22504,7 @@
       <c r="Y784" s="6"/>
       <c r="Z784" s="6"/>
     </row>
-    <row r="785" spans="1:26" ht="30" customHeight="1">
+    <row r="785" spans="1:26" ht="14">
       <c r="A785" s="7"/>
       <c r="B785" s="8"/>
       <c r="C785" s="9"/>
@@ -22644,7 +22644,7 @@
       <c r="Y789" s="6"/>
       <c r="Z789" s="6"/>
     </row>
-    <row r="790" spans="1:26" ht="30" customHeight="1">
+    <row r="790" spans="1:26" ht="14">
       <c r="A790" s="7"/>
       <c r="B790" s="8"/>
       <c r="C790" s="9"/>
@@ -22700,7 +22700,7 @@
       <c r="Y791" s="6"/>
       <c r="Z791" s="6"/>
     </row>
-    <row r="792" spans="1:26" ht="30" customHeight="1">
+    <row r="792" spans="1:26" ht="14">
       <c r="A792" s="7"/>
       <c r="B792" s="8"/>
       <c r="C792" s="9"/>
@@ -22728,7 +22728,7 @@
       <c r="Y792" s="6"/>
       <c r="Z792" s="6"/>
     </row>
-    <row r="793" spans="1:26" ht="30" customHeight="1">
+    <row r="793" spans="1:26" ht="14">
       <c r="A793" s="7"/>
       <c r="B793" s="8"/>
       <c r="C793" s="9"/>
@@ -22756,7 +22756,7 @@
       <c r="Y793" s="6"/>
       <c r="Z793" s="6"/>
     </row>
-    <row r="794" spans="1:26" ht="30" customHeight="1">
+    <row r="794" spans="1:26" ht="14">
       <c r="A794" s="7"/>
       <c r="B794" s="8"/>
       <c r="C794" s="9"/>
@@ -22784,7 +22784,7 @@
       <c r="Y794" s="6"/>
       <c r="Z794" s="6"/>
     </row>
-    <row r="795" spans="1:26" ht="30" customHeight="1">
+    <row r="795" spans="1:26" ht="14">
       <c r="A795" s="7"/>
       <c r="B795" s="8"/>
       <c r="C795" s="9"/>
@@ -22812,7 +22812,7 @@
       <c r="Y795" s="6"/>
       <c r="Z795" s="6"/>
     </row>
-    <row r="796" spans="1:26" ht="30" customHeight="1">
+    <row r="796" spans="1:26" ht="14">
       <c r="A796" s="7"/>
       <c r="B796" s="8"/>
       <c r="C796" s="9"/>
@@ -22868,7 +22868,7 @@
       <c r="Y797" s="6"/>
       <c r="Z797" s="6"/>
     </row>
-    <row r="798" spans="1:26" ht="30" customHeight="1">
+    <row r="798" spans="1:26" ht="14">
       <c r="A798" s="7"/>
       <c r="B798" s="8"/>
       <c r="C798" s="9"/>
@@ -22924,7 +22924,7 @@
       <c r="Y799" s="6"/>
       <c r="Z799" s="6"/>
     </row>
-    <row r="800" spans="1:26" ht="30" customHeight="1">
+    <row r="800" spans="1:26" ht="14">
       <c r="A800" s="7"/>
       <c r="B800" s="8"/>
       <c r="C800" s="9"/>
@@ -23008,7 +23008,7 @@
       <c r="Y802" s="6"/>
       <c r="Z802" s="6"/>
     </row>
-    <row r="803" spans="1:26" ht="30" customHeight="1">
+    <row r="803" spans="1:26" ht="14">
       <c r="A803" s="12"/>
       <c r="B803" s="13"/>
       <c r="C803" s="14"/>
@@ -23036,7 +23036,7 @@
       <c r="Y803" s="6"/>
       <c r="Z803" s="6"/>
     </row>
-    <row r="804" spans="1:26" ht="30" customHeight="1">
+    <row r="804" spans="1:26" ht="14">
       <c r="A804" s="12"/>
       <c r="B804" s="13"/>
       <c r="C804" s="14"/>
@@ -23092,7 +23092,7 @@
       <c r="Y805" s="6"/>
       <c r="Z805" s="6"/>
     </row>
-    <row r="806" spans="1:26" ht="30" customHeight="1">
+    <row r="806" spans="1:26" ht="14">
       <c r="A806" s="7"/>
       <c r="B806" s="8"/>
       <c r="C806" s="9"/>
@@ -23120,7 +23120,7 @@
       <c r="Y806" s="6"/>
       <c r="Z806" s="6"/>
     </row>
-    <row r="807" spans="1:26" ht="30" customHeight="1">
+    <row r="807" spans="1:26" ht="14">
       <c r="A807" s="7"/>
       <c r="B807" s="8"/>
       <c r="C807" s="9"/>
@@ -23148,7 +23148,7 @@
       <c r="Y807" s="6"/>
       <c r="Z807" s="6"/>
     </row>
-    <row r="808" spans="1:26" ht="30" customHeight="1">
+    <row r="808" spans="1:26" ht="14">
       <c r="A808" s="7"/>
       <c r="B808" s="8"/>
       <c r="C808" s="9"/>
@@ -23176,7 +23176,7 @@
       <c r="Y808" s="6"/>
       <c r="Z808" s="6"/>
     </row>
-    <row r="809" spans="1:26" ht="30" customHeight="1">
+    <row r="809" spans="1:26" ht="14">
       <c r="A809" s="7"/>
       <c r="B809" s="8"/>
       <c r="C809" s="9"/>
@@ -23204,7 +23204,7 @@
       <c r="Y809" s="6"/>
       <c r="Z809" s="6"/>
     </row>
-    <row r="810" spans="1:26" ht="30" customHeight="1">
+    <row r="810" spans="1:26" ht="14">
       <c r="A810" s="7"/>
       <c r="B810" s="8"/>
       <c r="C810" s="9"/>
@@ -23260,7 +23260,7 @@
       <c r="Y811" s="6"/>
       <c r="Z811" s="6"/>
     </row>
-    <row r="812" spans="1:26" ht="30" customHeight="1">
+    <row r="812" spans="1:26" ht="14">
       <c r="A812" s="7"/>
       <c r="B812" s="8"/>
       <c r="C812" s="9"/>
@@ -23288,7 +23288,7 @@
       <c r="Y812" s="6"/>
       <c r="Z812" s="6"/>
     </row>
-    <row r="813" spans="1:26" ht="30" customHeight="1">
+    <row r="813" spans="1:26" ht="14">
       <c r="A813" s="7"/>
       <c r="B813" s="8"/>
       <c r="C813" s="9"/>
@@ -23344,7 +23344,7 @@
       <c r="Y814" s="6"/>
       <c r="Z814" s="6"/>
     </row>
-    <row r="815" spans="1:26" ht="30" customHeight="1">
+    <row r="815" spans="1:26" ht="14">
       <c r="A815" s="7"/>
       <c r="B815" s="8"/>
       <c r="C815" s="9"/>
@@ -23400,7 +23400,7 @@
       <c r="Y816" s="6"/>
       <c r="Z816" s="6"/>
     </row>
-    <row r="817" spans="1:26" ht="30" customHeight="1">
+    <row r="817" spans="1:26" ht="14">
       <c r="A817" s="7"/>
       <c r="B817" s="8"/>
       <c r="C817" s="9"/>
@@ -23428,7 +23428,7 @@
       <c r="Y817" s="6"/>
       <c r="Z817" s="6"/>
     </row>
-    <row r="818" spans="1:26" ht="30" customHeight="1">
+    <row r="818" spans="1:26" ht="14">
       <c r="A818" s="7"/>
       <c r="B818" s="8"/>
       <c r="C818" s="9"/>
@@ -23456,7 +23456,7 @@
       <c r="Y818" s="6"/>
       <c r="Z818" s="6"/>
     </row>
-    <row r="819" spans="1:26" ht="30" customHeight="1">
+    <row r="819" spans="1:26" ht="14">
       <c r="A819" s="7"/>
       <c r="B819" s="8"/>
       <c r="C819" s="9"/>
@@ -23512,7 +23512,7 @@
       <c r="Y820" s="6"/>
       <c r="Z820" s="6"/>
     </row>
-    <row r="821" spans="1:26" ht="30" customHeight="1">
+    <row r="821" spans="1:26" ht="14">
       <c r="A821" s="7"/>
       <c r="B821" s="8"/>
       <c r="C821" s="9"/>
@@ -23540,7 +23540,7 @@
       <c r="Y821" s="6"/>
       <c r="Z821" s="6"/>
     </row>
-    <row r="822" spans="1:26" ht="30" customHeight="1">
+    <row r="822" spans="1:26" ht="14">
       <c r="A822" s="7"/>
       <c r="B822" s="8"/>
       <c r="C822" s="9"/>
@@ -23568,7 +23568,7 @@
       <c r="Y822" s="6"/>
       <c r="Z822" s="6"/>
     </row>
-    <row r="823" spans="1:26" ht="30" customHeight="1">
+    <row r="823" spans="1:26" ht="14">
       <c r="A823" s="7"/>
       <c r="B823" s="8"/>
       <c r="C823" s="9"/>
@@ -23596,7 +23596,7 @@
       <c r="Y823" s="6"/>
       <c r="Z823" s="6"/>
     </row>
-    <row r="824" spans="1:26" ht="30" customHeight="1">
+    <row r="824" spans="1:26" ht="14">
       <c r="A824" s="7"/>
       <c r="B824" s="8"/>
       <c r="C824" s="9"/>
@@ -23624,7 +23624,7 @@
       <c r="Y824" s="6"/>
       <c r="Z824" s="6"/>
     </row>
-    <row r="825" spans="1:26" ht="30" customHeight="1">
+    <row r="825" spans="1:26" ht="14">
       <c r="A825" s="7"/>
       <c r="B825" s="8"/>
       <c r="C825" s="9"/>
@@ -23680,7 +23680,7 @@
       <c r="Y826" s="6"/>
       <c r="Z826" s="6"/>
     </row>
-    <row r="827" spans="1:26" ht="30" customHeight="1">
+    <row r="827" spans="1:26" ht="14">
       <c r="A827" s="7"/>
       <c r="B827" s="8"/>
       <c r="C827" s="9"/>
@@ -23708,7 +23708,7 @@
       <c r="Y827" s="6"/>
       <c r="Z827" s="6"/>
     </row>
-    <row r="828" spans="1:26" ht="30" customHeight="1">
+    <row r="828" spans="1:26" ht="14">
       <c r="A828" s="7"/>
       <c r="B828" s="8"/>
       <c r="C828" s="9"/>
@@ -23736,7 +23736,7 @@
       <c r="Y828" s="6"/>
       <c r="Z828" s="6"/>
     </row>
-    <row r="829" spans="1:26" ht="30" customHeight="1">
+    <row r="829" spans="1:26" ht="14">
       <c r="A829" s="7"/>
       <c r="B829" s="8"/>
       <c r="C829" s="9"/>
@@ -23792,7 +23792,7 @@
       <c r="Y830" s="6"/>
       <c r="Z830" s="6"/>
     </row>
-    <row r="831" spans="1:26" ht="30" customHeight="1">
+    <row r="831" spans="1:26" ht="14">
       <c r="A831" s="7"/>
       <c r="B831" s="8"/>
       <c r="C831" s="9"/>
@@ -23820,7 +23820,7 @@
       <c r="Y831" s="6"/>
       <c r="Z831" s="6"/>
     </row>
-    <row r="832" spans="1:26" ht="30" customHeight="1">
+    <row r="832" spans="1:26" ht="14">
       <c r="A832" s="7"/>
       <c r="B832" s="8"/>
       <c r="C832" s="9"/>
@@ -23876,7 +23876,7 @@
       <c r="Y833" s="6"/>
       <c r="Z833" s="6"/>
     </row>
-    <row r="834" spans="1:26" ht="30" customHeight="1">
+    <row r="834" spans="1:26" ht="14">
       <c r="A834" s="7"/>
       <c r="B834" s="8"/>
       <c r="C834" s="9"/>
@@ -23904,7 +23904,7 @@
       <c r="Y834" s="6"/>
       <c r="Z834" s="6"/>
     </row>
-    <row r="835" spans="1:26" ht="30" customHeight="1">
+    <row r="835" spans="1:26" ht="14">
       <c r="A835" s="7"/>
       <c r="B835" s="8"/>
       <c r="C835" s="9"/>
@@ -23960,7 +23960,7 @@
       <c r="Y836" s="6"/>
       <c r="Z836" s="6"/>
     </row>
-    <row r="837" spans="1:26" ht="30" customHeight="1">
+    <row r="837" spans="1:26" ht="14">
       <c r="A837" s="7"/>
       <c r="B837" s="8"/>
       <c r="C837" s="9"/>
@@ -23988,7 +23988,7 @@
       <c r="Y837" s="6"/>
       <c r="Z837" s="6"/>
     </row>
-    <row r="838" spans="1:26" ht="30" customHeight="1">
+    <row r="838" spans="1:26" ht="14">
       <c r="A838" s="7"/>
       <c r="B838" s="8"/>
       <c r="C838" s="9"/>
@@ -24016,7 +24016,7 @@
       <c r="Y838" s="6"/>
       <c r="Z838" s="6"/>
     </row>
-    <row r="839" spans="1:26" ht="30" customHeight="1">
+    <row r="839" spans="1:26" ht="14">
       <c r="A839" s="12"/>
       <c r="B839" s="13"/>
       <c r="C839" s="14"/>
@@ -24044,7 +24044,7 @@
       <c r="Y839" s="6"/>
       <c r="Z839" s="6"/>
     </row>
-    <row r="840" spans="1:26" ht="30" customHeight="1">
+    <row r="840" spans="1:26" ht="14">
       <c r="A840" s="7"/>
       <c r="B840" s="8"/>
       <c r="C840" s="9"/>
@@ -24072,7 +24072,7 @@
       <c r="Y840" s="6"/>
       <c r="Z840" s="6"/>
     </row>
-    <row r="841" spans="1:26" ht="30" customHeight="1">
+    <row r="841" spans="1:26" ht="14">
       <c r="A841" s="7"/>
       <c r="B841" s="8"/>
       <c r="C841" s="9"/>
@@ -24100,7 +24100,7 @@
       <c r="Y841" s="6"/>
       <c r="Z841" s="6"/>
     </row>
-    <row r="842" spans="1:26" ht="30" customHeight="1">
+    <row r="842" spans="1:26" ht="14">
       <c r="A842" s="7"/>
       <c r="B842" s="8"/>
       <c r="C842" s="9"/>
@@ -24128,7 +24128,7 @@
       <c r="Y842" s="6"/>
       <c r="Z842" s="6"/>
     </row>
-    <row r="843" spans="1:26" ht="30" customHeight="1">
+    <row r="843" spans="1:26" ht="14">
       <c r="A843" s="7"/>
       <c r="B843" s="8"/>
       <c r="C843" s="9"/>
@@ -24156,7 +24156,7 @@
       <c r="Y843" s="6"/>
       <c r="Z843" s="6"/>
     </row>
-    <row r="844" spans="1:26" ht="30" customHeight="1">
+    <row r="844" spans="1:26" ht="14">
       <c r="A844" s="7"/>
       <c r="B844" s="8"/>
       <c r="C844" s="9"/>
@@ -24184,7 +24184,7 @@
       <c r="Y844" s="6"/>
       <c r="Z844" s="6"/>
     </row>
-    <row r="845" spans="1:26" ht="30" customHeight="1">
+    <row r="845" spans="1:26" ht="14">
       <c r="A845" s="7"/>
       <c r="B845" s="8"/>
       <c r="C845" s="9"/>
@@ -24212,7 +24212,7 @@
       <c r="Y845" s="6"/>
       <c r="Z845" s="6"/>
     </row>
-    <row r="846" spans="1:26" ht="30" customHeight="1">
+    <row r="846" spans="1:26" ht="14">
       <c r="A846" s="7"/>
       <c r="B846" s="8"/>
       <c r="C846" s="9"/>
@@ -24324,7 +24324,7 @@
       <c r="Y849" s="6"/>
       <c r="Z849" s="6"/>
     </row>
-    <row r="850" spans="1:26" ht="30" customHeight="1">
+    <row r="850" spans="1:26" ht="14">
       <c r="A850" s="7"/>
       <c r="B850" s="8"/>
       <c r="C850" s="9"/>
@@ -24352,7 +24352,7 @@
       <c r="Y850" s="6"/>
       <c r="Z850" s="6"/>
     </row>
-    <row r="851" spans="1:26" ht="30" customHeight="1">
+    <row r="851" spans="1:26" ht="14">
       <c r="A851" s="7"/>
       <c r="B851" s="8"/>
       <c r="C851" s="9"/>
@@ -24464,7 +24464,7 @@
       <c r="Y854" s="6"/>
       <c r="Z854" s="6"/>
     </row>
-    <row r="855" spans="1:26" ht="30" customHeight="1">
+    <row r="855" spans="1:26" ht="14">
       <c r="A855" s="7"/>
       <c r="B855" s="8"/>
       <c r="C855" s="9"/>
@@ -24520,7 +24520,7 @@
       <c r="Y856" s="6"/>
       <c r="Z856" s="6"/>
     </row>
-    <row r="857" spans="1:26" ht="30" customHeight="1">
+    <row r="857" spans="1:26" ht="14">
       <c r="A857" s="7"/>
       <c r="B857" s="8"/>
       <c r="C857" s="9"/>
@@ -24548,7 +24548,7 @@
       <c r="Y857" s="6"/>
       <c r="Z857" s="6"/>
     </row>
-    <row r="858" spans="1:26" ht="30" customHeight="1">
+    <row r="858" spans="1:26" ht="14">
       <c r="A858" s="7"/>
       <c r="B858" s="8"/>
       <c r="C858" s="9"/>
@@ -24576,7 +24576,7 @@
       <c r="Y858" s="6"/>
       <c r="Z858" s="6"/>
     </row>
-    <row r="859" spans="1:26" ht="30" customHeight="1">
+    <row r="859" spans="1:26" ht="14">
       <c r="A859" s="7"/>
       <c r="B859" s="8"/>
       <c r="C859" s="9"/>
@@ -24604,7 +24604,7 @@
       <c r="Y859" s="6"/>
       <c r="Z859" s="6"/>
     </row>
-    <row r="860" spans="1:26" ht="30" customHeight="1">
+    <row r="860" spans="1:26" ht="14">
       <c r="A860" s="7"/>
       <c r="B860" s="8"/>
       <c r="C860" s="9"/>
@@ -24632,7 +24632,7 @@
       <c r="Y860" s="6"/>
       <c r="Z860" s="6"/>
     </row>
-    <row r="861" spans="1:26" ht="30" customHeight="1">
+    <row r="861" spans="1:26" ht="14">
       <c r="A861" s="7"/>
       <c r="B861" s="8"/>
       <c r="C861" s="9"/>
@@ -24660,7 +24660,7 @@
       <c r="Y861" s="6"/>
       <c r="Z861" s="6"/>
     </row>
-    <row r="862" spans="1:26" ht="30" customHeight="1">
+    <row r="862" spans="1:26" ht="14">
       <c r="A862" s="7"/>
       <c r="B862" s="8"/>
       <c r="C862" s="9"/>
@@ -24688,7 +24688,7 @@
       <c r="Y862" s="6"/>
       <c r="Z862" s="6"/>
     </row>
-    <row r="863" spans="1:26" ht="30" customHeight="1">
+    <row r="863" spans="1:26" ht="14">
       <c r="A863" s="7"/>
       <c r="B863" s="8"/>
       <c r="C863" s="9"/>
@@ -24772,7 +24772,7 @@
       <c r="Y865" s="6"/>
       <c r="Z865" s="6"/>
     </row>
-    <row r="866" spans="1:26" ht="30" customHeight="1">
+    <row r="866" spans="1:26" ht="14">
       <c r="A866" s="7"/>
       <c r="B866" s="8"/>
       <c r="C866" s="9"/>
@@ -24800,7 +24800,7 @@
       <c r="Y866" s="6"/>
       <c r="Z866" s="6"/>
     </row>
-    <row r="867" spans="1:26" ht="30" customHeight="1">
+    <row r="867" spans="1:26" ht="14">
       <c r="A867" s="7"/>
       <c r="B867" s="8"/>
       <c r="C867" s="9"/>
@@ -24828,7 +24828,7 @@
       <c r="Y867" s="6"/>
       <c r="Z867" s="6"/>
     </row>
-    <row r="868" spans="1:26" ht="30" customHeight="1">
+    <row r="868" spans="1:26" ht="14">
       <c r="A868" s="7"/>
       <c r="B868" s="8"/>
       <c r="C868" s="9"/>
@@ -24884,7 +24884,7 @@
       <c r="Y869" s="6"/>
       <c r="Z869" s="6"/>
     </row>
-    <row r="870" spans="1:26" ht="30" customHeight="1">
+    <row r="870" spans="1:26" ht="14">
       <c r="A870" s="7"/>
       <c r="B870" s="8"/>
       <c r="C870" s="9"/>
@@ -24912,7 +24912,7 @@
       <c r="Y870" s="6"/>
       <c r="Z870" s="6"/>
     </row>
-    <row r="871" spans="1:26" ht="30" customHeight="1">
+    <row r="871" spans="1:26" ht="14">
       <c r="A871" s="7"/>
       <c r="B871" s="8"/>
       <c r="C871" s="9"/>
@@ -24940,7 +24940,7 @@
       <c r="Y871" s="6"/>
       <c r="Z871" s="6"/>
     </row>
-    <row r="872" spans="1:26" ht="30" customHeight="1">
+    <row r="872" spans="1:26" ht="14">
       <c r="A872" s="7"/>
       <c r="B872" s="8"/>
       <c r="C872" s="9"/>
@@ -24996,7 +24996,7 @@
       <c r="Y873" s="6"/>
       <c r="Z873" s="6"/>
     </row>
-    <row r="874" spans="1:26" ht="30" customHeight="1">
+    <row r="874" spans="1:26" ht="14">
       <c r="A874" s="7"/>
       <c r="B874" s="8"/>
       <c r="C874" s="9"/>
@@ -25024,7 +25024,7 @@
       <c r="Y874" s="6"/>
       <c r="Z874" s="6"/>
     </row>
-    <row r="875" spans="1:26" ht="30" customHeight="1">
+    <row r="875" spans="1:26" ht="14">
       <c r="A875" s="7"/>
       <c r="B875" s="8"/>
       <c r="C875" s="9"/>
@@ -25052,7 +25052,7 @@
       <c r="Y875" s="6"/>
       <c r="Z875" s="6"/>
     </row>
-    <row r="876" spans="1:26" ht="30" customHeight="1">
+    <row r="876" spans="1:26" ht="14">
       <c r="A876" s="12"/>
       <c r="B876" s="13"/>
       <c r="C876" s="14"/>
@@ -25080,7 +25080,7 @@
       <c r="Y876" s="6"/>
       <c r="Z876" s="6"/>
     </row>
-    <row r="877" spans="1:26" ht="30" customHeight="1">
+    <row r="877" spans="1:26" ht="14">
       <c r="A877" s="12"/>
       <c r="B877" s="13"/>
       <c r="C877" s="14"/>
@@ -25108,7 +25108,7 @@
       <c r="Y877" s="6"/>
       <c r="Z877" s="6"/>
     </row>
-    <row r="878" spans="1:26" ht="30" customHeight="1">
+    <row r="878" spans="1:26" ht="14">
       <c r="A878" s="12"/>
       <c r="B878" s="13"/>
       <c r="C878" s="14"/>
@@ -25192,7 +25192,7 @@
       <c r="Y880" s="6"/>
       <c r="Z880" s="6"/>
     </row>
-    <row r="881" spans="1:26" ht="30" customHeight="1">
+    <row r="881" spans="1:26" ht="14">
       <c r="A881" s="12"/>
       <c r="B881" s="13"/>
       <c r="C881" s="14"/>
@@ -25248,7 +25248,7 @@
       <c r="Y882" s="6"/>
       <c r="Z882" s="6"/>
     </row>
-    <row r="883" spans="1:26" ht="30" customHeight="1">
+    <row r="883" spans="1:26" ht="14">
       <c r="A883" s="7"/>
       <c r="B883" s="8"/>
       <c r="C883" s="9"/>
@@ -25276,7 +25276,7 @@
       <c r="Y883" s="6"/>
       <c r="Z883" s="6"/>
     </row>
-    <row r="884" spans="1:26" ht="30" customHeight="1">
+    <row r="884" spans="1:26" ht="14">
       <c r="A884" s="7"/>
       <c r="B884" s="8"/>
       <c r="C884" s="9"/>
@@ -25360,7 +25360,7 @@
       <c r="Y886" s="6"/>
       <c r="Z886" s="6"/>
     </row>
-    <row r="887" spans="1:26" ht="30" customHeight="1">
+    <row r="887" spans="1:26" ht="14">
       <c r="A887" s="7"/>
       <c r="B887" s="8"/>
       <c r="C887" s="9"/>
@@ -25388,7 +25388,7 @@
       <c r="Y887" s="6"/>
       <c r="Z887" s="6"/>
     </row>
-    <row r="888" spans="1:26" ht="30" customHeight="1">
+    <row r="888" spans="1:26" ht="14">
       <c r="A888" s="7"/>
       <c r="B888" s="8"/>
       <c r="C888" s="9"/>
@@ -25416,7 +25416,7 @@
       <c r="Y888" s="6"/>
       <c r="Z888" s="6"/>
     </row>
-    <row r="889" spans="1:26" ht="30" customHeight="1">
+    <row r="889" spans="1:26" ht="14">
       <c r="A889" s="7"/>
       <c r="B889" s="8"/>
       <c r="C889" s="9"/>
@@ -25556,7 +25556,7 @@
       <c r="Y893" s="6"/>
       <c r="Z893" s="6"/>
     </row>
-    <row r="894" spans="1:26" ht="30" customHeight="1">
+    <row r="894" spans="1:26" ht="14">
       <c r="A894" s="12"/>
       <c r="B894" s="13"/>
       <c r="C894" s="14"/>
@@ -25612,7 +25612,7 @@
       <c r="Y895" s="6"/>
       <c r="Z895" s="6"/>
     </row>
-    <row r="896" spans="1:26" ht="30" customHeight="1">
+    <row r="896" spans="1:26" ht="14">
       <c r="A896" s="12"/>
       <c r="B896" s="13"/>
       <c r="C896" s="14"/>
@@ -25640,7 +25640,7 @@
       <c r="Y896" s="6"/>
       <c r="Z896" s="6"/>
     </row>
-    <row r="897" spans="1:26" ht="30" customHeight="1">
+    <row r="897" spans="1:26" ht="14">
       <c r="A897" s="12"/>
       <c r="B897" s="13"/>
       <c r="C897" s="14"/>
@@ -25668,7 +25668,7 @@
       <c r="Y897" s="6"/>
       <c r="Z897" s="6"/>
     </row>
-    <row r="898" spans="1:26" ht="30" customHeight="1">
+    <row r="898" spans="1:26" ht="14">
       <c r="A898" s="7"/>
       <c r="B898" s="8"/>
       <c r="C898" s="9"/>
@@ -25696,7 +25696,7 @@
       <c r="Y898" s="6"/>
       <c r="Z898" s="6"/>
     </row>
-    <row r="899" spans="1:26" ht="30" customHeight="1">
+    <row r="899" spans="1:26" ht="14">
       <c r="A899" s="7"/>
       <c r="B899" s="8"/>
       <c r="C899" s="9"/>
@@ -25808,7 +25808,7 @@
       <c r="Y902" s="6"/>
       <c r="Z902" s="6"/>
     </row>
-    <row r="903" spans="1:26" ht="30" customHeight="1">
+    <row r="903" spans="1:26" ht="14">
       <c r="A903" s="7"/>
       <c r="B903" s="8"/>
       <c r="C903" s="9"/>
@@ -25836,7 +25836,7 @@
       <c r="Y903" s="6"/>
       <c r="Z903" s="6"/>
     </row>
-    <row r="904" spans="1:26" ht="30" customHeight="1">
+    <row r="904" spans="1:26" ht="14">
       <c r="A904" s="7"/>
       <c r="B904" s="8"/>
       <c r="C904" s="9"/>
@@ -25976,7 +25976,7 @@
       <c r="Y908" s="6"/>
       <c r="Z908" s="6"/>
     </row>
-    <row r="909" spans="1:26" ht="30" customHeight="1">
+    <row r="909" spans="1:26" ht="14">
       <c r="A909" s="7"/>
       <c r="B909" s="8"/>
       <c r="C909" s="9"/>
@@ -26004,7 +26004,7 @@
       <c r="Y909" s="6"/>
       <c r="Z909" s="6"/>
     </row>
-    <row r="910" spans="1:26" ht="30" customHeight="1">
+    <row r="910" spans="1:26" ht="14">
       <c r="A910" s="7"/>
       <c r="B910" s="8"/>
       <c r="C910" s="9"/>
@@ -26032,7 +26032,7 @@
       <c r="Y910" s="6"/>
       <c r="Z910" s="6"/>
     </row>
-    <row r="911" spans="1:26" ht="30" customHeight="1">
+    <row r="911" spans="1:26" ht="14">
       <c r="A911" s="7"/>
       <c r="B911" s="8"/>
       <c r="C911" s="9"/>
@@ -26116,7 +26116,7 @@
       <c r="Y913" s="6"/>
       <c r="Z913" s="6"/>
     </row>
-    <row r="914" spans="1:26" ht="30" customHeight="1">
+    <row r="914" spans="1:26" ht="14">
       <c r="A914" s="12"/>
       <c r="B914" s="13"/>
       <c r="C914" s="14"/>
@@ -26144,7 +26144,7 @@
       <c r="Y914" s="6"/>
       <c r="Z914" s="6"/>
     </row>
-    <row r="915" spans="1:26" ht="30" customHeight="1">
+    <row r="915" spans="1:26" ht="14">
       <c r="A915" s="12"/>
       <c r="B915" s="13"/>
       <c r="C915" s="14"/>
@@ -26172,7 +26172,7 @@
       <c r="Y915" s="6"/>
       <c r="Z915" s="6"/>
     </row>
-    <row r="916" spans="1:26" ht="30" customHeight="1">
+    <row r="916" spans="1:26" ht="14">
       <c r="A916" s="12"/>
       <c r="B916" s="13"/>
       <c r="C916" s="14"/>
@@ -26228,7 +26228,7 @@
       <c r="Y917" s="6"/>
       <c r="Z917" s="6"/>
     </row>
-    <row r="918" spans="1:26" ht="30" customHeight="1">
+    <row r="918" spans="1:26" ht="14">
       <c r="A918" s="12"/>
       <c r="B918" s="13"/>
       <c r="C918" s="14"/>
@@ -26256,7 +26256,7 @@
       <c r="Y918" s="6"/>
       <c r="Z918" s="6"/>
     </row>
-    <row r="919" spans="1:26" ht="30" customHeight="1">
+    <row r="919" spans="1:26" ht="14">
       <c r="A919" s="12"/>
       <c r="B919" s="13"/>
       <c r="C919" s="14"/>
@@ -26284,7 +26284,7 @@
       <c r="Y919" s="6"/>
       <c r="Z919" s="6"/>
     </row>
-    <row r="920" spans="1:26" ht="30" customHeight="1">
+    <row r="920" spans="1:26" ht="14">
       <c r="A920" s="12"/>
       <c r="B920" s="13"/>
       <c r="C920" s="14"/>
@@ -26312,7 +26312,7 @@
       <c r="Y920" s="6"/>
       <c r="Z920" s="6"/>
     </row>
-    <row r="921" spans="1:26" ht="30" customHeight="1">
+    <row r="921" spans="1:26" ht="14">
       <c r="A921" s="12"/>
       <c r="B921" s="13"/>
       <c r="C921" s="14"/>
@@ -26368,7 +26368,7 @@
       <c r="Y922" s="6"/>
       <c r="Z922" s="6"/>
     </row>
-    <row r="923" spans="1:26" ht="30" customHeight="1">
+    <row r="923" spans="1:26" ht="14">
       <c r="A923" s="12"/>
       <c r="B923" s="13"/>
       <c r="C923" s="14"/>

</xml_diff>